<commit_message>
started draft iptds implementation plan
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3282A67-C8CC-49E4-B728-31AC4EA552E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A283C-2011-4B21-88B8-EEECE886A5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O&amp;M Costs" sheetId="1" r:id="rId1"/>
@@ -2333,10 +2333,10 @@
   <dimension ref="A1:AG61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG62" sqref="AG62"/>
+      <selection pane="bottomRight" activeCell="AG60" sqref="AG60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -8343,7 +8343,7 @@
         <v>18370</v>
       </c>
       <c r="T53" s="19">
-        <f t="shared" ref="S53:X53" si="43">SUMIFS(T$2:T$49,$D$2:$D$49,$Q53,T$2:T$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="T53:X53" si="43">SUMIFS(T$2:T$49,$D$2:$D$49,$Q53,T$2:T$49,"&lt;&gt;#N/A")</f>
         <v>163900</v>
       </c>
       <c r="U53" s="19">
@@ -8380,7 +8380,7 @@
         <v>26580</v>
       </c>
       <c r="AD53" s="21">
-        <f t="shared" ref="AC53:AE53" si="44">SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q53,AD$2:AD$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AD53:AE53" si="44">SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q53,AD$2:AD$49,"&lt;&gt;#N/A")</f>
         <v>22505.100000000002</v>
       </c>
       <c r="AE53" s="21">
@@ -8405,7 +8405,7 @@
         <v>13142</v>
       </c>
       <c r="S54" s="19">
-        <f t="shared" ref="R54:Y56" si="45">SUMIFS(S$2:S$49,$D$2:$D$49,$Q54,S$2:S$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="S54:X56" si="45">SUMIFS(S$2:S$49,$D$2:$D$49,$Q54,S$2:S$49,"&lt;&gt;#N/A")</f>
         <v>7515</v>
       </c>
       <c r="T54" s="19">
@@ -8603,7 +8603,7 @@
         <v>50904</v>
       </c>
       <c r="S58" s="47">
-        <f t="shared" ref="S58:AG58" si="47">S53+S56</f>
+        <f t="shared" ref="S58:AE58" si="47">S53+S56</f>
         <v>24215</v>
       </c>
       <c r="T58" s="47">
@@ -8669,7 +8669,7 @@
         <v>59078</v>
       </c>
       <c r="S59" s="47">
-        <f t="shared" ref="S59:AG59" si="48">SUM(S53:S55)</f>
+        <f t="shared" ref="S59:AE59" si="48">SUM(S53:S55)</f>
         <v>29225</v>
       </c>
       <c r="T59" s="47">
@@ -8735,7 +8735,7 @@
         <v>8174</v>
       </c>
       <c r="S60" s="47">
-        <f t="shared" ref="S60:AG60" si="49">S59-S58</f>
+        <f t="shared" ref="S60:AE60" si="49">S59-S58</f>
         <v>5010</v>
       </c>
       <c r="T60" s="47">
@@ -8801,7 +8801,7 @@
         <v>0.16057677196291056</v>
       </c>
       <c r="S61" s="52">
-        <f t="shared" ref="S61:AG61" si="50">S60/S58</f>
+        <f t="shared" ref="S61:AE61" si="50">S60/S58</f>
         <v>0.20689655172413793</v>
       </c>
       <c r="T61" s="52">

</xml_diff>

<commit_message>
saving o&m costs; updated Rstudio
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A283C-2011-4B21-88B8-EEECE886A5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D5FD2D-B656-49CE-B054-0D83AF1F29A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O&amp;M Costs" sheetId="1" r:id="rId1"/>
@@ -2333,10 +2333,10 @@
   <dimension ref="A1:AG61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG60" sqref="AG60"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -15453,7 +15453,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1048576"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
minor updates to implementation plan and o&m costs
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11801219-2F3E-45D2-B66B-0F7A1D2DC895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D6E5C-82EE-461B-85D9-C84A95B3353F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proponent Costs" sheetId="4" r:id="rId1"/>
@@ -2466,7 +2466,7 @@
   <dimension ref="B2:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.35"/>
@@ -2728,10 +2728,10 @@
   <dimension ref="A1:AI61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI61" sqref="AI61"/>
+      <selection pane="bottomRight" activeCell="AE48" sqref="AE48:AG48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed site codes for ESS/ZEN A0 & B0
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D6E5C-82EE-461B-85D9-C84A95B3353F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1EED4D-0837-4696-A1D4-E1E7F272D741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proponent Costs" sheetId="4" r:id="rId1"/>
@@ -2465,23 +2465,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6A41C-4EE9-4E25-91C6-882C326C1FB9}">
   <dimension ref="B2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.453125" style="98" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" style="93" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.1796875" style="108" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" style="95" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="98" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="98" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" style="93" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.21875" style="108" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="95" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="98" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="98" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="98" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="98"/>
+    <col min="9" max="16384" width="8.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="92" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" s="92" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B2" s="88" t="s">
         <v>371</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="B3" s="93" t="s">
         <v>369</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>65439.679999999993</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="93" t="s">
         <v>7</v>
       </c>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="2:11" s="107" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" s="107" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="104" t="s">
         <v>374</v>
       </c>
@@ -2727,53 +2727,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE48" sqref="AE48:AG48"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.08984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.453125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" style="85" customWidth="1"/>
-    <col min="9" max="9" width="20.54296875" style="85" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.453125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.54296875" style="31" customWidth="1"/>
-    <col min="12" max="12" width="17.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.08984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="85" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" style="85" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" style="31" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.21875" style="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.26953125" style="16" customWidth="1"/>
-    <col min="20" max="20" width="11.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.08984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.90625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.1796875" style="25" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.90625" style="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.7265625" style="26" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.90625" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.1796875" style="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.54296875" style="21" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.1796875" style="27" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1796875" style="28" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7265625" style="17"/>
+    <col min="18" max="18" width="7.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" style="16" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.77734375" style="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.21875" style="27" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.21875" style="28" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="8" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>233</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C10" s="18" t="b">
         <v>1</v>
@@ -4056,7 +4056,7 @@
         <v>237</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C11" s="18" t="b">
         <v>1</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>330</v>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="P12" s="16">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q12" s="17" t="str">
         <f t="shared" si="4"/>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="X12" s="19">
         <f t="shared" si="11"/>
-        <v>17610</v>
+        <v>11740</v>
       </c>
       <c r="Y12" s="19">
         <f t="shared" si="12"/>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="AA12" s="20">
         <f t="shared" si="20"/>
-        <v>53324</v>
+        <v>47454</v>
       </c>
       <c r="AB12" s="39">
         <f t="shared" si="14"/>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="AC12" s="20">
         <f t="shared" si="21"/>
-        <v>5332.4000000000005</v>
+        <v>4745.4000000000005</v>
       </c>
       <c r="AD12" s="21">
         <f t="shared" si="15"/>
@@ -4310,12 +4310,12 @@
       </c>
       <c r="AI12" s="23">
         <f t="shared" si="22"/>
-        <v>9776.7800000000007</v>
+        <v>9189.7800000000007</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>331</v>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="P13" s="16">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="17" t="str">
         <f t="shared" si="4"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="X13" s="19">
         <f t="shared" si="11"/>
-        <v>11740</v>
+        <v>17610</v>
       </c>
       <c r="Y13" s="19">
         <f t="shared" si="12"/>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="AA13" s="20">
         <f t="shared" si="20"/>
-        <v>47454</v>
+        <v>53324</v>
       </c>
       <c r="AB13" s="39">
         <f t="shared" si="14"/>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="AC13" s="20">
         <f t="shared" si="21"/>
-        <v>4745.4000000000005</v>
+        <v>5332.4000000000005</v>
       </c>
       <c r="AD13" s="21">
         <f t="shared" si="15"/>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="AI13" s="23">
         <f t="shared" si="22"/>
-        <v>9189.7800000000007</v>
+        <v>9776.7800000000007</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
@@ -8976,7 +8976,7 @@
       <c r="J50" s="18"/>
       <c r="K50" s="29"/>
     </row>
-    <row r="52" spans="1:35" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S52" s="40" t="s">
         <v>354</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>59439.7</v>
       </c>
     </row>
-    <row r="58" spans="1:35" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S58" s="33" t="s">
         <v>355</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>280203.15999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:35" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S59" s="33" t="s">
         <v>356</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>345642.83999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S60" s="33" t="s">
         <v>357</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>65439.679999999993</v>
       </c>
     </row>
-    <row r="61" spans="1:35" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S61" s="33" t="s">
         <v>359</v>
       </c>
@@ -9576,61 +9576,61 @@
       <selection sqref="A1:AW1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.90625" style="71" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="71" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="71" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" style="71" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1796875" style="71" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" style="71" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="62" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="62" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" style="62" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" style="62" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="71" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" style="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" style="71" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="71" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="71" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="71" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="71" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="62" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="62" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.08984375" style="62" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="62" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="62" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="62" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.90625" style="62" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1796875" style="62" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="62" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.21875" style="62" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="62" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.453125" style="62" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.90625" style="62" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.26953125" style="62" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.54296875" style="62" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.26953125" style="62" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.36328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.453125" style="62" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.54296875" style="62" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.1796875" style="62" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.36328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.1796875" style="62" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.1796875" style="62" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.08984375" style="62" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.90625" style="62" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.08984375" style="62" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.26953125" style="62" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.36328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.6328125" style="62" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" style="62" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" style="62" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.5546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.33203125" style="62" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.88671875" style="62" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.21875" style="62" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.33203125" style="62" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.6640625" style="62" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="13" style="62" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.7265625" style="62" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.36328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.90625" style="62" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.81640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.77734375" style="62" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.33203125" style="62" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.88671875" style="62" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.77734375" style="62" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="11" style="62" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" style="62" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.1796875" style="62" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.21875" style="62" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="8" style="62" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.54296875" style="62" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.81640625" style="62" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="8.7265625" style="62"/>
+    <col min="48" max="48" width="7.5546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.77734375" style="62" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="8.77734375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>103</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
         <v>9</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>6956.5</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
         <v>11</v>
       </c>
@@ -10061,7 +10061,7 @@
         <v>10403.99</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>13</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>6472.8</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
         <v>15</v>
       </c>
@@ -10341,7 +10341,7 @@
         <v>6277.7</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6" s="58" t="s">
         <v>31</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>6508.88</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7" s="58" t="s">
         <v>43</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>9725.19</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A8" s="58" t="s">
         <v>37</v>
       </c>
@@ -10758,7 +10758,7 @@
         <v>9272.7800000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9" s="58" t="s">
         <v>90</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>8685.7800000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
         <v>83</v>
       </c>
@@ -11032,7 +11032,7 @@
         <v>7348.7800000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" s="58" t="s">
         <v>86</v>
       </c>
@@ -11173,7 +11173,7 @@
         <v>10403.99</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12" s="58" t="s">
         <v>88</v>
       </c>
@@ -11314,7 +11314,7 @@
         <v>10697.49</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13" s="58" t="s">
         <v>92</v>
       </c>
@@ -11455,7 +11455,7 @@
         <v>7543.5</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A14" s="58" t="s">
         <v>51</v>
       </c>
@@ -11596,7 +11596,7 @@
         <v>15240.72</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A15" s="58" t="s">
         <v>54</v>
       </c>
@@ -11723,7 +11723,7 @@
         <v>11478.83</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A16" s="58" t="s">
         <v>233</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>8685.7800000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A17" s="58" t="s">
         <v>237</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>8685.7800000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A18" s="58" t="s">
         <v>49</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>12348.67</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A19" s="58" t="s">
         <v>47</v>
       </c>
@@ -12273,7 +12273,7 @@
         <v>11204.91</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A20" s="58" t="s">
         <v>242</v>
       </c>
@@ -12418,7 +12418,7 @@
         <v>9776.7800000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A21" s="58" t="s">
         <v>246</v>
       </c>
@@ -12563,7 +12563,7 @@
         <v>9189.7800000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A22" s="58" t="s">
         <v>250</v>
       </c>
@@ -12700,7 +12700,7 @@
         <v>7543.5</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A23" s="58" t="s">
         <v>257</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>7311.92</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A24" s="58" t="s">
         <v>259</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>7543.5</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A25" s="58" t="s">
         <v>263</v>
       </c>
@@ -13113,7 +13113,7 @@
         <v>7543.5</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A26" s="58" t="s">
         <v>266</v>
       </c>
@@ -13246,7 +13246,7 @@
         <v>5392</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A27" s="58" t="s">
         <v>270</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>6277.7</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A28" s="58" t="s">
         <v>275</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>8258.98</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A29" s="58" t="s">
         <v>279</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>10134.5</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A30" s="58" t="s">
         <v>283</v>
       </c>
@@ -13798,7 +13798,7 @@
         <v>6277.7</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A31" s="58" t="s">
         <v>286</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>6025.7</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A32" s="58" t="s">
         <v>290</v>
       </c>
@@ -14070,7 +14070,7 @@
         <v>8510.98</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A33" s="58" t="s">
         <v>293</v>
       </c>
@@ -14207,7 +14207,7 @@
         <v>8258.98</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A34" s="58" t="s">
         <v>62</v>
       </c>
@@ -14338,7 +14338,7 @@
         <v>3442.4</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A35" s="58" t="s">
         <v>70</v>
       </c>
@@ -14473,7 +14473,7 @@
         <v>4289.12</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A36" s="58" t="s">
         <v>72</v>
       </c>
@@ -14602,7 +14602,7 @@
         <v>3984.32</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A37" s="58" t="s">
         <v>64</v>
       </c>
@@ -14741,7 +14741,7 @@
         <v>5268.24</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A38" s="58" t="s">
         <v>60</v>
       </c>
@@ -14884,7 +14884,7 @@
         <v>6071.28</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A39" s="58" t="s">
         <v>68</v>
       </c>
@@ -15023,7 +15023,7 @@
         <v>3509.2</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A40" s="58" t="s">
         <v>66</v>
       </c>
@@ -15166,7 +15166,7 @@
         <v>5903.5</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A41" s="58" t="s">
         <v>74</v>
       </c>
@@ -15303,7 +15303,7 @@
         <v>8006.9800000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A42" s="58" t="s">
         <v>76</v>
       </c>
@@ -15444,7 +15444,7 @@
         <v>6277.7</v>
       </c>
     </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A43" s="58" t="s">
         <v>80</v>
       </c>
@@ -15585,7 +15585,7 @@
         <v>9977.9500000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A44" s="58" t="s">
         <v>17</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>10233.76</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A45" s="58" t="s">
         <v>19</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>12642.880000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A46" s="58" t="s">
         <v>58</v>
       </c>
@@ -16006,7 +16006,7 @@
         <v>7245.12</v>
       </c>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A47" s="58" t="s">
         <v>29</v>
       </c>
@@ -16155,18 +16155,18 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="72" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" style="72" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.54296875" style="73" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" style="72" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.5546875" style="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>341</v>
       </c>
@@ -16183,7 +16183,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>343</v>
       </c>
@@ -16200,7 +16200,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>131</v>
       </c>
@@ -16217,7 +16217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>155</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>344</v>
       </c>
@@ -16251,7 +16251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>348</v>
       </c>
@@ -16261,7 +16261,7 @@
       <c r="E7" s="79"/>
       <c r="F7" s="77"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E8" s="75" t="s">
         <v>137</v>
       </c>
@@ -16269,7 +16269,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D9" s="73"/>
       <c r="E9" s="7" t="s">
         <v>333</v>
@@ -16278,7 +16278,7 @@
         <v>3121</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D10" s="73"/>
       <c r="E10" s="7" t="s">
         <v>334</v>
@@ -16287,7 +16287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D11" s="73"/>
       <c r="E11" s="7" t="s">
         <v>360</v>
@@ -16296,7 +16296,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D12" s="73"/>
       <c r="E12" s="7" t="s">
         <v>335</v>
@@ -16305,7 +16305,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E13" s="5" t="s">
         <v>174</v>
       </c>
@@ -16313,8 +16313,8 @@
         <v>835</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E15" s="75" t="s">
         <v>136</v>
       </c>
@@ -16322,7 +16322,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E16" s="7" t="s">
         <v>173</v>
       </c>
@@ -16330,7 +16330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E17" s="7" t="s">
         <v>192</v>
       </c>
@@ -16338,7 +16338,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E18" s="5" t="s">
         <v>340</v>
       </c>
@@ -16346,8 +16346,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="19" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="75" t="s">
         <v>336</v>
       </c>
@@ -16355,7 +16355,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="7" t="s">
         <v>172</v>
       </c>
@@ -16363,7 +16363,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E22" s="7" t="s">
         <v>191</v>
       </c>
@@ -16371,7 +16371,7 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E23" s="7" t="s">
         <v>337</v>
       </c>
@@ -16379,7 +16379,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="5" t="s">
         <v>338</v>
       </c>
@@ -16387,8 +16387,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="25" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E26" s="80" t="s">
         <v>346</v>
       </c>
@@ -16399,7 +16399,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E27" s="7" t="s">
         <v>165</v>
       </c>
@@ -16410,7 +16410,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E28" s="7" t="s">
         <v>320</v>
       </c>
@@ -16421,7 +16421,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E29" s="7" t="s">
         <v>183</v>
       </c>
@@ -16432,7 +16432,7 @@
         <v>780.19</v>
       </c>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E30" s="7" t="s">
         <v>207</v>
       </c>
@@ -16443,7 +16443,7 @@
         <v>1560.38</v>
       </c>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E31" s="7" t="s">
         <v>230</v>
       </c>
@@ -16454,7 +16454,7 @@
         <v>3120.75</v>
       </c>
     </row>
-    <row r="32" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E32" s="5" t="s">
         <v>224</v>
       </c>

</xml_diff>

<commit_message>
just saving o&m costs
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1EED4D-0837-4696-A1D4-E1E7F272D741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD1A39A-400B-4DD6-B9FB-0E949EBF9250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2466,7 +2466,7 @@
   <dimension ref="B2:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
re-folded ACM back into o&m costs, map
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD1A39A-400B-4DD6-B9FB-0E949EBF9250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3595E02D-847A-43BC-A6F6-844C82AF2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proponent Costs" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Fixed Costs" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'O&amp;M Costs'!$A$1:$AI$62</definedName>
     <definedName name="antenna_cost">'Fixed Costs'!$C$3</definedName>
     <definedName name="battery_cost">'Fixed Costs'!$C$4</definedName>
     <definedName name="battery_replacement">'Fixed Costs'!$C$5</definedName>
@@ -287,7 +288,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="L37" authorId="24" shapeId="0" xr:uid="{34D9FD0C-C923-4A9F-949B-12953991A15C}">
+    <comment ref="L38" authorId="24" shapeId="0" xr:uid="{34D9FD0C-C923-4A9F-949B-12953991A15C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -295,7 +296,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="P37" authorId="25" shapeId="0" xr:uid="{AE9481D7-4476-403B-8541-16BCB964FA37}">
+    <comment ref="P38" authorId="25" shapeId="0" xr:uid="{AE9481D7-4476-403B-8541-16BCB964FA37}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -303,7 +304,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="Q37" authorId="26" shapeId="0" xr:uid="{544378C6-124C-4C92-A642-0AE43F3F3061}">
+    <comment ref="Q38" authorId="26" shapeId="0" xr:uid="{544378C6-124C-4C92-A642-0AE43F3F3061}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -311,7 +312,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="R37" authorId="27" shapeId="0" xr:uid="{00E8D40E-04F4-4F93-AB45-467AF4CC9362}">
+    <comment ref="R38" authorId="27" shapeId="0" xr:uid="{00E8D40E-04F4-4F93-AB45-467AF4CC9362}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -319,7 +320,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="L38" authorId="28" shapeId="0" xr:uid="{351259EF-3985-4698-AF5C-40B4E8213980}">
+    <comment ref="L39" authorId="28" shapeId="0" xr:uid="{351259EF-3985-4698-AF5C-40B4E8213980}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +328,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="P38" authorId="29" shapeId="0" xr:uid="{ED26637F-FBCE-4F79-8C43-FED7D517BFB2}">
+    <comment ref="P39" authorId="29" shapeId="0" xr:uid="{ED26637F-FBCE-4F79-8C43-FED7D517BFB2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -335,7 +336,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="Q38" authorId="30" shapeId="0" xr:uid="{4DDFA2D5-BA85-40F5-B9BE-AFB3430867B9}">
+    <comment ref="Q39" authorId="30" shapeId="0" xr:uid="{4DDFA2D5-BA85-40F5-B9BE-AFB3430867B9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -343,7 +344,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="R38" authorId="31" shapeId="0" xr:uid="{29297ED3-A1F8-45DB-8894-83E4684C9CB7}">
+    <comment ref="R39" authorId="31" shapeId="0" xr:uid="{29297ED3-A1F8-45DB-8894-83E4684C9CB7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -351,7 +352,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="P39" authorId="32" shapeId="0" xr:uid="{EFDEDEC3-3251-49D7-B8F8-775B538E2941}">
+    <comment ref="P40" authorId="32" shapeId="0" xr:uid="{EFDEDEC3-3251-49D7-B8F8-775B538E2941}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -359,7 +360,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="Q39" authorId="33" shapeId="0" xr:uid="{B5188D8D-C0C6-4175-87BE-772A73E6CB11}">
+    <comment ref="Q40" authorId="33" shapeId="0" xr:uid="{B5188D8D-C0C6-4175-87BE-772A73E6CB11}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -367,7 +368,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="R39" authorId="34" shapeId="0" xr:uid="{66CA20A2-0F08-4F4D-90A2-5C0926FD9D3D}">
+    <comment ref="R40" authorId="34" shapeId="0" xr:uid="{66CA20A2-0F08-4F4D-90A2-5C0926FD9D3D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -375,7 +376,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="S39" authorId="35" shapeId="0" xr:uid="{9D013F0B-84F0-4B8C-8916-5524E19E2129}">
+    <comment ref="S40" authorId="35" shapeId="0" xr:uid="{9D013F0B-84F0-4B8C-8916-5524E19E2129}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -383,7 +384,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="P40" authorId="36" shapeId="0" xr:uid="{7813689E-9B6F-49FC-A9B2-338961C7EFC4}">
+    <comment ref="P41" authorId="36" shapeId="0" xr:uid="{7813689E-9B6F-49FC-A9B2-338961C7EFC4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -391,7 +392,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="Q40" authorId="37" shapeId="0" xr:uid="{692E4B72-3AF6-49DC-AA12-A6D2E4057EDD}">
+    <comment ref="Q41" authorId="37" shapeId="0" xr:uid="{692E4B72-3AF6-49DC-AA12-A6D2E4057EDD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -399,7 +400,7 @@
     Guesstimate</t>
       </text>
     </comment>
-    <comment ref="R40" authorId="38" shapeId="0" xr:uid="{0BC2EF01-7A2F-4F3D-AE49-65515A710650}">
+    <comment ref="R41" authorId="38" shapeId="0" xr:uid="{0BC2EF01-7A2F-4F3D-AE49-65515A710650}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -412,7 +413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="391">
   <si>
     <t>WDFW</t>
   </si>
@@ -1539,9 +1540,6 @@
     <t>Totals:</t>
   </si>
   <si>
-    <t>PCA, YFK, SW1, SW2, SC4, LAP, WR2, MR1, WEN, USC, USP, CHA, LSR</t>
-  </si>
-  <si>
     <t>USI, CAC, BTL, LLS, BHC, SFG, BSC, COC, IR2</t>
   </si>
   <si>
@@ -1570,6 +1568,24 @@
   </si>
   <si>
     <t>Diff. Total O&amp;M Costs</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>Candidate to transfer to project</t>
+  </si>
+  <si>
+    <t>Asotin Creek near mouth</t>
+  </si>
+  <si>
+    <t>PSMFC</t>
+  </si>
+  <si>
+    <t>NOAA, PSMFC</t>
+  </si>
+  <si>
+    <t>PCA, YFK, SW1, SW2, SC4, LAP, WR2, MR1, WEN, USC, USP, CHA, LSR, ACM</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1826,7 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2049,6 +2065,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2413,49 +2444,49 @@
   <threadedComment ref="R36" dT="2024-08-14T19:33:14.09" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{2A5E4EEF-D24F-449E-BB01-A08A33121190}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="L37" dT="2024-08-14T19:35:46.76" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{34D9FD0C-C923-4A9F-949B-12953991A15C}">
+  <threadedComment ref="L38" dT="2024-08-14T19:35:46.76" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{34D9FD0C-C923-4A9F-949B-12953991A15C}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="P37" dT="2024-08-14T19:36:58.45" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{AE9481D7-4476-403B-8541-16BCB964FA37}">
+  <threadedComment ref="P38" dT="2024-08-14T19:36:58.45" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{AE9481D7-4476-403B-8541-16BCB964FA37}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="Q37" dT="2024-08-14T19:37:07.31" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{544378C6-124C-4C92-A642-0AE43F3F3061}">
+  <threadedComment ref="Q38" dT="2024-08-14T19:37:07.31" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{544378C6-124C-4C92-A642-0AE43F3F3061}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="R37" dT="2024-08-14T19:37:14.89" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{00E8D40E-04F4-4F93-AB45-467AF4CC9362}">
+  <threadedComment ref="R38" dT="2024-08-14T19:37:14.89" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{00E8D40E-04F4-4F93-AB45-467AF4CC9362}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="L38" dT="2024-08-14T19:37:51.25" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{351259EF-3985-4698-AF5C-40B4E8213980}">
+  <threadedComment ref="L39" dT="2024-08-14T19:37:51.25" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{351259EF-3985-4698-AF5C-40B4E8213980}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="P38" dT="2024-08-14T19:37:58.83" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{ED26637F-FBCE-4F79-8C43-FED7D517BFB2}">
+  <threadedComment ref="P39" dT="2024-08-14T19:37:58.83" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{ED26637F-FBCE-4F79-8C43-FED7D517BFB2}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="Q38" dT="2024-08-14T19:38:06.04" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{4DDFA2D5-BA85-40F5-B9BE-AFB3430867B9}">
+  <threadedComment ref="Q39" dT="2024-08-14T19:38:06.04" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{4DDFA2D5-BA85-40F5-B9BE-AFB3430867B9}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="R38" dT="2024-08-14T19:38:14.61" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{29297ED3-A1F8-45DB-8894-83E4684C9CB7}">
+  <threadedComment ref="R39" dT="2024-08-14T19:38:14.61" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{29297ED3-A1F8-45DB-8894-83E4684C9CB7}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="P39" dT="2024-08-14T19:45:05.01" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{EFDEDEC3-3251-49D7-B8F8-775B538E2941}">
+  <threadedComment ref="P40" dT="2024-08-14T19:45:05.01" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{EFDEDEC3-3251-49D7-B8F8-775B538E2941}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="Q39" dT="2024-08-14T19:45:12.52" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{B5188D8D-C0C6-4175-87BE-772A73E6CB11}">
+  <threadedComment ref="Q40" dT="2024-08-14T19:45:12.52" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{B5188D8D-C0C6-4175-87BE-772A73E6CB11}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="R39" dT="2024-08-14T19:45:20.67" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{66CA20A2-0F08-4F4D-90A2-5C0926FD9D3D}">
+  <threadedComment ref="R40" dT="2024-08-14T19:45:20.67" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{66CA20A2-0F08-4F4D-90A2-5C0926FD9D3D}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="S39" dT="2024-08-14T19:45:33.23" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{9D013F0B-84F0-4B8C-8916-5524E19E2129}">
+  <threadedComment ref="S40" dT="2024-08-14T19:45:33.23" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{9D013F0B-84F0-4B8C-8916-5524E19E2129}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="P40" dT="2024-08-14T19:46:40.04" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{7813689E-9B6F-49FC-A9B2-338961C7EFC4}">
+  <threadedComment ref="P41" dT="2024-08-14T19:46:40.04" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{7813689E-9B6F-49FC-A9B2-338961C7EFC4}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="Q40" dT="2024-08-14T19:46:49.76" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{692E4B72-3AF6-49DC-AA12-A6D2E4057EDD}">
+  <threadedComment ref="Q41" dT="2024-08-14T19:46:49.76" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{692E4B72-3AF6-49DC-AA12-A6D2E4057EDD}">
     <text>Guesstimate</text>
   </threadedComment>
-  <threadedComment ref="R40" dT="2024-08-14T19:46:57.56" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{0BC2EF01-7A2F-4F3D-AE49-65515A710650}">
+  <threadedComment ref="R41" dT="2024-08-14T19:46:57.56" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{0BC2EF01-7A2F-4F3D-AE49-65515A710650}">
     <text>Guesstimate</text>
   </threadedComment>
 </ThreadedComments>
@@ -2463,10 +2494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6A41C-4EE9-4E25-91C6-882C326C1FB9}">
-  <dimension ref="B2:K21"/>
+  <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2492,16 +2523,16 @@
         <v>373</v>
       </c>
       <c r="E2" s="90" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F2" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="G2" s="91" t="s">
         <v>383</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="H2" s="91" t="s">
         <v>384</v>
-      </c>
-      <c r="H2" s="91" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
@@ -2509,25 +2540,25 @@
         <v>369</v>
       </c>
       <c r="C3" s="94" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" s="94" t="s">
         <v>375</v>
       </c>
-      <c r="D3" s="94" t="s">
-        <v>376</v>
-      </c>
       <c r="E3" s="95">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="96">
-        <f>SUMIF('O&amp;M Costs'!$H$2:$H$49,B3,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>280203.16000000003</v>
       </c>
       <c r="G3" s="96">
-        <f>SUMIF('O&amp;M Costs'!$I$2:$I$49,B3,'O&amp;M Costs'!$AI$2:$AI$49)</f>
-        <v>345642.84</v>
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>351238.12000000005</v>
       </c>
       <c r="H3" s="97">
         <f>G3-F3</f>
-        <v>65439.679999999993</v>
+        <v>71034.960000000021</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -2535,20 +2566,20 @@
         <v>7</v>
       </c>
       <c r="C4" s="94" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="94" t="s">
         <v>378</v>
-      </c>
-      <c r="D4" s="94" t="s">
-        <v>379</v>
       </c>
       <c r="E4" s="95">
         <v>-4</v>
       </c>
       <c r="F4" s="96">
-        <f>SUMIF('O&amp;M Costs'!$H$2:$H$49,B4,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>66249.05</v>
       </c>
       <c r="G4" s="96">
-        <f>SUMIF('O&amp;M Costs'!$I$2:$I$49,B4,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>27343.010000000002</v>
       </c>
       <c r="H4" s="97">
@@ -2561,7 +2592,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="94" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D5" s="94" t="s">
         <v>34</v>
@@ -2570,11 +2601,11 @@
         <v>-1</v>
       </c>
       <c r="F5" s="96">
-        <f>SUMIF('O&amp;M Costs'!$H$2:$H$49,B5,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B5,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>6910.4</v>
       </c>
       <c r="G5" s="96">
-        <f>SUMIF('O&amp;M Costs'!$I$2:$I$49,B5,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B5,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>0</v>
       </c>
       <c r="H5" s="97">
@@ -2588,20 +2619,20 @@
         <v>53</v>
       </c>
       <c r="C6" s="94" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="94" t="s">
         <v>380</v>
-      </c>
-      <c r="D6" s="94" t="s">
-        <v>381</v>
       </c>
       <c r="E6" s="95">
         <v>-2</v>
       </c>
       <c r="F6" s="96">
-        <f>SUMIF('O&amp;M Costs'!$H$2:$H$49,B6,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>14239.119999999999</v>
       </c>
       <c r="G6" s="96">
-        <f>SUMIF('O&amp;M Costs'!$I$2:$I$49,B6,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>0</v>
       </c>
       <c r="H6" s="97">
@@ -2611,65 +2642,85 @@
       <c r="K6" s="16"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="109" t="s">
         <v>370</v>
       </c>
-      <c r="C7" s="100" t="s">
-        <v>382</v>
-      </c>
-      <c r="D7" s="100" t="s">
-        <v>380</v>
-      </c>
-      <c r="E7" s="101">
+      <c r="C7" s="110" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" s="110" t="s">
+        <v>379</v>
+      </c>
+      <c r="E7" s="111">
         <v>4</v>
       </c>
-      <c r="F7" s="102">
-        <f>SUMIF('O&amp;M Costs'!$H$2:$H$49,B7,'O&amp;M Costs'!$AI$2:$AI$49)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="102">
-        <f>SUMIF('O&amp;M Costs'!$I$2:$I$49,B7,'O&amp;M Costs'!$AI$2:$AI$49)</f>
+      <c r="F7" s="112">
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="112">
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
         <v>15225.039999999999</v>
       </c>
-      <c r="H7" s="103">
+      <c r="H7" s="113">
         <f t="shared" si="0"/>
         <v>15225.039999999999</v>
       </c>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="2:11" s="107" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100" t="s">
+        <v>385</v>
+      </c>
+      <c r="E8" s="101">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="102">
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>5595.2800000000007</v>
+      </c>
+      <c r="G8" s="102">
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="103">
+        <f t="shared" ref="H8" si="1">G8-F8</f>
+        <v>-5595.2800000000007</v>
+      </c>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="2:11" s="107" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="104" t="s">
         <v>374</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="105">
-        <f>SUM(E3:E7)</f>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="105">
+        <f>SUM(E3:E8)</f>
         <v>1</v>
       </c>
-      <c r="F8" s="106">
-        <f>SUM(F3:F7)</f>
-        <v>367601.73000000004</v>
-      </c>
-      <c r="G8" s="106">
-        <f>SUM(G3:G7)</f>
-        <v>388210.89</v>
-      </c>
-      <c r="H8" s="106">
-        <f>SUM(H3:H7)</f>
-        <v>20609.159999999989</v>
-      </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K9" s="16"/>
+      <c r="F9" s="106">
+        <f>SUM(F3:F8)</f>
+        <v>373197.01000000007</v>
+      </c>
+      <c r="G9" s="106">
+        <f>SUM(G3:G8)</f>
+        <v>393806.17000000004</v>
+      </c>
+      <c r="H9" s="106">
+        <f>SUM(H3:H8)</f>
+        <v>20609.160000000018</v>
+      </c>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K10" s="16"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -2689,7 +2740,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D15" s="16"/>
-      <c r="E15" s="87"/>
+      <c r="E15" s="16"/>
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
@@ -2705,6 +2756,7 @@
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D18" s="16"/>
       <c r="E18" s="87"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D19" s="16"/>
@@ -2718,6 +2770,10 @@
       <c r="D21" s="16"/>
       <c r="E21" s="87"/>
     </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D22" s="16"/>
+      <c r="E22" s="87"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2725,13 +2781,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI61"/>
+  <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="AH38" sqref="AH38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2999,7 +3055,7 @@
         <v>3120.75</v>
       </c>
       <c r="AG2" s="21">
-        <f t="shared" ref="AG2:AG49" si="18">data_management_mnth*12</f>
+        <f t="shared" ref="AG2:AG50" si="18">data_management_mnth*12</f>
         <v>1080</v>
       </c>
       <c r="AH2" s="22">
@@ -3106,7 +3162,7 @@
         <v>12500</v>
       </c>
       <c r="AA3" s="20">
-        <f t="shared" ref="AA3:AA48" si="20">SUM(T3:Z3)</f>
+        <f t="shared" ref="AA3:AA49" si="20">SUM(T3:Z3)</f>
         <v>52591</v>
       </c>
       <c r="AB3" s="39">
@@ -3114,7 +3170,7 @@
         <v>0.08</v>
       </c>
       <c r="AC3" s="20">
-        <f t="shared" ref="AC3:AC48" si="21">AA3*AB3</f>
+        <f t="shared" ref="AC3:AC49" si="21">AA3*AB3</f>
         <v>4207.28</v>
       </c>
       <c r="AD3" s="21">
@@ -3138,7 +3194,7 @@
         <v>1864</v>
       </c>
       <c r="AI3" s="23">
-        <f t="shared" ref="AI3:AI48" si="22">AH3+AC3</f>
+        <f t="shared" ref="AI3:AI49" si="22">AH3+AC3</f>
         <v>6071.28</v>
       </c>
     </row>
@@ -3523,7 +3579,7 @@
         <v>1080</v>
       </c>
       <c r="AH6" s="22">
-        <f t="shared" ref="AH6:AH48" si="23">SUM(AD6:AG6)</f>
+        <f t="shared" ref="AH6:AH49" si="23">SUM(AD6:AG6)</f>
         <v>3004</v>
       </c>
       <c r="AI6" s="23">
@@ -5214,7 +5270,7 @@
         <v>120</v>
       </c>
       <c r="AG19" s="21">
-        <f t="shared" ref="AG19:AG48" si="25">data_management_mnth*12</f>
+        <f t="shared" ref="AG19:AG49" si="25">data_management_mnth*12</f>
         <v>1080</v>
       </c>
       <c r="AH19" s="22">
@@ -6928,27 +6984,27 @@
         <v>0</v>
       </c>
       <c r="T33" s="19">
-        <f t="shared" ref="T33:T48" si="26">VLOOKUP(L33,communication,2,FALSE)</f>
+        <f t="shared" ref="T33:T49" si="26">VLOOKUP(L33,communication,2,FALSE)</f>
         <v>742</v>
       </c>
       <c r="U33" s="19">
-        <f t="shared" ref="U33:U48" si="27">IFERROR(VLOOKUP(M33,datalogger,2,FALSE),0)</f>
+        <f t="shared" ref="U33:U49" si="27">IFERROR(VLOOKUP(M33,datalogger,2,FALSE),0)</f>
         <v>835</v>
       </c>
       <c r="V33" s="19">
-        <f t="shared" ref="V33:V48" si="28">IFERROR(VLOOKUP(N33,transceiver,2,FALSE),0)</f>
+        <f t="shared" ref="V33:V49" si="28">IFERROR(VLOOKUP(N33,transceiver,2,FALSE),0)</f>
         <v>4450</v>
       </c>
       <c r="W33" s="19">
-        <f t="shared" ref="W33:W48" si="29">VLOOKUP(O33,reader,2,FALSE)*P33</f>
+        <f t="shared" ref="W33:W49" si="29">VLOOKUP(O33,reader,2,FALSE)*P33</f>
         <v>8336</v>
       </c>
       <c r="X33" s="19">
-        <f t="shared" ref="X33:X48" si="30">P33*antenna_cost</f>
+        <f t="shared" ref="X33:X49" si="30">P33*antenna_cost</f>
         <v>11740</v>
       </c>
       <c r="Y33" s="19">
-        <f t="shared" ref="Y33:Y48" si="31">_xlfn.IFS(Q33="Grid Power", 2550, Q33="Grid Power PLC", 3940, Q33="5060 Hybrid TEG", 27903, Q33="5060 TEG", 10479, Q33="5120 TEG", 13874, Q33="Solar", solar_array_cost*S33)+(R33*battery_cost)</f>
+        <f t="shared" ref="Y33:Y49" si="31">_xlfn.IFS(Q33="Grid Power", 2550, Q33="Grid Power PLC", 3940, Q33="5060 Hybrid TEG", 27903, Q33="5060 TEG", 10479, Q33="5120 TEG", 13874, Q33="Solar", solar_array_cost*S33)+(R33*battery_cost)</f>
         <v>3950</v>
       </c>
       <c r="Z33" s="38">
@@ -6966,15 +7022,15 @@
         <v>3404.2400000000002</v>
       </c>
       <c r="AD33" s="21">
-        <f t="shared" ref="AD33:AD48" si="32">(R33*battery_replacement)/4</f>
+        <f t="shared" ref="AD33:AD49" si="32">(R33*battery_replacement)/4</f>
         <v>364</v>
       </c>
       <c r="AE33" s="21">
-        <f t="shared" ref="AE33:AE48" si="33">VLOOKUP(L33,communication,3,FALSE)</f>
+        <f t="shared" ref="AE33:AE49" si="33">VLOOKUP(L33,communication,3,FALSE)</f>
         <v>300</v>
       </c>
       <c r="AF33" s="21">
-        <f t="shared" ref="AF33:AF48" si="34">VLOOKUP(Q33,power,3,FALSE)</f>
+        <f t="shared" ref="AF33:AF49" si="34">VLOOKUP(Q33,power,3,FALSE)</f>
         <v>120</v>
       </c>
       <c r="AG33" s="21">
@@ -7355,34 +7411,40 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>101</v>
+        <v>387</v>
       </c>
       <c r="C37" s="18" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>97</v>
+        <v>386</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="86" t="s">
-        <v>363</v>
-      </c>
-      <c r="I37" s="86" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="85" t="s">
         <v>369</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="K37" s="30"/>
+        <v>388</v>
+      </c>
+      <c r="K37" s="30" t="s">
+        <v>389</v>
+      </c>
       <c r="L37" s="57" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="M37" s="57" t="s">
         <v>174</v>
@@ -7394,86 +7456,86 @@
         <v>192</v>
       </c>
       <c r="P37" s="83">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Q37" s="57" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="R37" s="83">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S37" s="83">
         <v>0</v>
       </c>
       <c r="T37" s="19">
-        <f t="shared" si="26"/>
-        <v>2000</v>
+        <f t="shared" ref="T37" si="35">VLOOKUP(L37,communication,2,FALSE)</f>
+        <v>742</v>
       </c>
       <c r="U37" s="19">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="U37" si="36">IFERROR(VLOOKUP(M37,datalogger,2,FALSE),0)</f>
         <v>835</v>
       </c>
       <c r="V37" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="V37" si="37">IFERROR(VLOOKUP(N37,transceiver,2,FALSE),0)</f>
         <v>4450</v>
       </c>
       <c r="W37" s="19">
-        <f t="shared" si="29"/>
-        <v>25008</v>
+        <f t="shared" ref="W37" si="38">VLOOKUP(O37,reader,2,FALSE)*P37</f>
+        <v>12504</v>
       </c>
       <c r="X37" s="19">
-        <f t="shared" si="30"/>
-        <v>35220</v>
+        <f t="shared" ref="X37" si="39">P37*antenna_cost</f>
+        <v>17610</v>
       </c>
       <c r="Y37" s="19">
-        <f t="shared" si="31"/>
-        <v>15274</v>
+        <f t="shared" ref="Y37" si="40">_xlfn.IFS(Q37="Grid Power", 2550, Q37="Grid Power PLC", 3940, Q37="5060 Hybrid TEG", 27903, Q37="5060 TEG", 10479, Q37="5120 TEG", 13874, Q37="Solar", solar_array_cost*S37)+(R37*battery_cost)</f>
+        <v>2550</v>
       </c>
       <c r="Z37" s="38">
         <v>12500</v>
       </c>
       <c r="AA37" s="20">
-        <f t="shared" si="20"/>
-        <v>95287</v>
+        <f t="shared" ref="AA37" si="41">SUM(T37:Z37)</f>
+        <v>51191</v>
       </c>
       <c r="AB37" s="39">
         <v>0.08</v>
       </c>
       <c r="AC37" s="20">
-        <f t="shared" si="21"/>
-        <v>7622.96</v>
+        <f t="shared" ref="AC37" si="42">AA37*AB37</f>
+        <v>4095.28</v>
       </c>
       <c r="AD37" s="21">
-        <f t="shared" si="32"/>
-        <v>364</v>
+        <f t="shared" ref="AD37" si="43">(R37*battery_replacement)/4</f>
+        <v>0</v>
       </c>
       <c r="AE37" s="21">
-        <f t="shared" si="33"/>
-        <v>1440</v>
+        <f t="shared" ref="AE37" si="44">VLOOKUP(L37,communication,3,FALSE)</f>
+        <v>300</v>
       </c>
       <c r="AF37" s="21">
-        <f t="shared" si="34"/>
-        <v>3120.75</v>
+        <f t="shared" ref="AF37" si="45">VLOOKUP(Q37,power,3,FALSE)</f>
+        <v>120</v>
       </c>
       <c r="AG37" s="21">
         <f t="shared" si="25"/>
         <v>1080</v>
       </c>
       <c r="AH37" s="22">
-        <f t="shared" si="23"/>
-        <v>6004.75</v>
+        <f>SUM(AD37:AG37)</f>
+        <v>1500</v>
       </c>
       <c r="AI37" s="23">
-        <f t="shared" si="22"/>
-        <v>13627.71</v>
+        <f t="shared" ref="AI37" si="46">AH37+AC37</f>
+        <v>5595.2800000000007</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="18" t="b">
         <v>0</v>
@@ -7585,10 +7647,10 @@
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>95</v>
+        <v>365</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="18" t="b">
         <v>0</v>
@@ -7624,16 +7686,16 @@
         <v>192</v>
       </c>
       <c r="P39" s="83">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q39" s="57" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="R39" s="83">
         <v>4</v>
       </c>
       <c r="S39" s="83">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T39" s="19">
         <f t="shared" si="26"/>
@@ -7649,29 +7711,29 @@
       </c>
       <c r="W39" s="19">
         <f t="shared" si="29"/>
-        <v>16672</v>
+        <v>25008</v>
       </c>
       <c r="X39" s="19">
         <f t="shared" si="30"/>
-        <v>23480</v>
+        <v>35220</v>
       </c>
       <c r="Y39" s="19">
         <f t="shared" si="31"/>
-        <v>29303</v>
+        <v>15274</v>
       </c>
       <c r="Z39" s="38">
         <v>12500</v>
       </c>
       <c r="AA39" s="20">
         <f t="shared" si="20"/>
-        <v>89240</v>
+        <v>95287</v>
       </c>
       <c r="AB39" s="39">
         <v>0.08</v>
       </c>
       <c r="AC39" s="20">
         <f t="shared" si="21"/>
-        <v>7139.2</v>
+        <v>7622.96</v>
       </c>
       <c r="AD39" s="21">
         <f t="shared" si="32"/>
@@ -7683,7 +7745,7 @@
       </c>
       <c r="AF39" s="21">
         <f t="shared" si="34"/>
-        <v>780.19</v>
+        <v>3120.75</v>
       </c>
       <c r="AG39" s="21">
         <f t="shared" si="25"/>
@@ -7691,19 +7753,19 @@
       </c>
       <c r="AH39" s="22">
         <f t="shared" si="23"/>
-        <v>3664.19</v>
+        <v>6004.75</v>
       </c>
       <c r="AI39" s="23">
         <f t="shared" si="22"/>
-        <v>10803.39</v>
+        <v>13627.71</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C40" s="18" t="b">
         <v>0</v>
@@ -7727,7 +7789,7 @@
       </c>
       <c r="K40" s="30"/>
       <c r="L40" s="57" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="M40" s="57" t="s">
         <v>174</v>
@@ -7742,17 +7804,17 @@
         <v>8</v>
       </c>
       <c r="Q40" s="57" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="R40" s="83">
         <v>4</v>
       </c>
       <c r="S40" s="83">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T40" s="19">
         <f t="shared" si="26"/>
-        <v>742</v>
+        <v>2000</v>
       </c>
       <c r="U40" s="19">
         <f t="shared" si="27"/>
@@ -7772,21 +7834,21 @@
       </c>
       <c r="Y40" s="19">
         <f t="shared" si="31"/>
-        <v>3950</v>
+        <v>29303</v>
       </c>
       <c r="Z40" s="38">
         <v>12500</v>
       </c>
       <c r="AA40" s="20">
         <f t="shared" si="20"/>
-        <v>62629</v>
+        <v>89240</v>
       </c>
       <c r="AB40" s="39">
         <v>0.08</v>
       </c>
       <c r="AC40" s="20">
         <f t="shared" si="21"/>
-        <v>5010.32</v>
+        <v>7139.2</v>
       </c>
       <c r="AD40" s="21">
         <f t="shared" si="32"/>
@@ -7794,11 +7856,11 @@
       </c>
       <c r="AE40" s="21">
         <f t="shared" si="33"/>
-        <v>300</v>
+        <v>1440</v>
       </c>
       <c r="AF40" s="21">
         <f t="shared" si="34"/>
-        <v>120</v>
+        <v>780.19</v>
       </c>
       <c r="AG40" s="21">
         <f t="shared" si="25"/>
@@ -7806,77 +7868,63 @@
       </c>
       <c r="AH40" s="22">
         <f t="shared" si="23"/>
-        <v>1864</v>
+        <v>3664.19</v>
       </c>
       <c r="AI40" s="23">
         <f t="shared" si="22"/>
-        <v>6874.32</v>
+        <v>10803.39</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="C41" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="86" t="s">
+        <v>363</v>
+      </c>
+      <c r="I41" s="86" t="s">
+        <v>369</v>
+      </c>
+      <c r="J41" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="K41" s="30"/>
+      <c r="L41" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="M41" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="N41" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="O41" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="P41" s="83">
         <v>8</v>
       </c>
-      <c r="G41" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="H41" s="85" t="s">
-        <v>369</v>
-      </c>
-      <c r="I41" s="85" t="s">
-        <v>363</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K41" s="29" t="s">
-        <v>362</v>
-      </c>
-      <c r="L41" s="17" t="str">
-        <f t="shared" ref="L41:L48" si="35">VLOOKUP(A41,om_table,23,FALSE)</f>
-        <v>Cellular Modem</v>
-      </c>
-      <c r="M41" s="17" t="str">
-        <f>VLOOKUP(A41,om_table,22,FALSE)</f>
-        <v>BioProbe3</v>
-      </c>
-      <c r="N41" s="17" t="str">
-        <f>VLOOKUP(A41,om_table,20,FALSE)</f>
-        <v>FS1001M</v>
-      </c>
-      <c r="O41" s="57" t="str">
-        <f t="shared" ref="O41:O48" si="36">VLOOKUP(A41,om_table,21,FALSE)</f>
-        <v>Biomark MUX</v>
-      </c>
-      <c r="P41" s="16">
-        <f t="shared" ref="P41:P48" si="37">VLOOKUP(A41,om_table,30,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="Q41" s="17" t="str">
-        <f t="shared" ref="Q41:Q48" si="38">VLOOKUP(A41,om_table,9,FALSE)</f>
-        <v>Grid Power</v>
-      </c>
-      <c r="R41" s="16">
-        <f t="shared" ref="R41:R48" si="39">VLOOKUP(A41,om_table,16,FALSE)</f>
+      <c r="Q41" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="R41" s="83">
         <v>4</v>
       </c>
-      <c r="S41" s="16">
-        <f t="shared" ref="S41:S48" si="40">VLOOKUP(A41,om_table,17,FALSE)</f>
+      <c r="S41" s="83">
         <v>0</v>
       </c>
       <c r="T41" s="19">
@@ -7889,35 +7937,33 @@
       </c>
       <c r="V41" s="19">
         <f t="shared" si="28"/>
-        <v>8500</v>
+        <v>4450</v>
       </c>
       <c r="W41" s="19">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>16672</v>
       </c>
       <c r="X41" s="19">
         <f t="shared" si="30"/>
-        <v>17610</v>
+        <v>23480</v>
       </c>
       <c r="Y41" s="19">
         <f t="shared" si="31"/>
         <v>3950</v>
       </c>
-      <c r="Z41" s="19">
-        <f t="shared" ref="Z41:Z48" si="41">VLOOKUP(A41,om_table,40,FALSE)</f>
+      <c r="Z41" s="38">
         <v>12500</v>
       </c>
       <c r="AA41" s="20">
         <f t="shared" si="20"/>
-        <v>44137</v>
+        <v>62629</v>
       </c>
       <c r="AB41" s="39">
-        <f t="shared" ref="AB41:AB48" si="42">VLOOKUP(A41,om_table,48,FALSE)</f>
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="AC41" s="20">
         <f t="shared" si="21"/>
-        <v>4413.7</v>
+        <v>5010.32</v>
       </c>
       <c r="AD41" s="21">
         <f t="shared" si="32"/>
@@ -7941,15 +7987,15 @@
       </c>
       <c r="AI41" s="23">
         <f t="shared" si="22"/>
-        <v>6277.7</v>
+        <v>6874.32</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C42" s="18" t="b">
         <v>1</v>
@@ -7970,7 +8016,7 @@
         <v>369</v>
       </c>
       <c r="I42" s="85" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="J42" s="18" t="s">
         <v>1</v>
@@ -7979,28 +8025,36 @@
         <v>362</v>
       </c>
       <c r="L42" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="L42:L49" si="47">VLOOKUP(A42,om_table,23,FALSE)</f>
         <v>Cellular Modem</v>
       </c>
+      <c r="M42" s="17" t="str">
+        <f>VLOOKUP(A42,om_table,22,FALSE)</f>
+        <v>BioProbe3</v>
+      </c>
+      <c r="N42" s="17" t="str">
+        <f>VLOOKUP(A42,om_table,20,FALSE)</f>
+        <v>FS1001M</v>
+      </c>
       <c r="O42" s="57" t="str">
-        <f t="shared" si="36"/>
-        <v>Biomark IS1001</v>
+        <f t="shared" ref="O42:O49" si="48">VLOOKUP(A42,om_table,21,FALSE)</f>
+        <v>Biomark MUX</v>
       </c>
       <c r="P42" s="16">
-        <f t="shared" si="37"/>
-        <v>2</v>
+        <f t="shared" ref="P42:P49" si="49">VLOOKUP(A42,om_table,30,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="Q42" s="17" t="str">
-        <f t="shared" si="38"/>
-        <v>Solar</v>
+        <f t="shared" ref="Q42:Q49" si="50">VLOOKUP(A42,om_table,9,FALSE)</f>
+        <v>Grid Power</v>
       </c>
       <c r="R42" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="R42:R49" si="51">VLOOKUP(A42,om_table,16,FALSE)</f>
         <v>4</v>
       </c>
       <c r="S42" s="16">
-        <f t="shared" si="40"/>
-        <v>4</v>
+        <f t="shared" ref="S42:S49" si="52">VLOOKUP(A42,om_table,17,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="T42" s="19">
         <f t="shared" si="26"/>
@@ -8008,39 +8062,39 @@
       </c>
       <c r="U42" s="19">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>835</v>
       </c>
       <c r="V42" s="19">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>8500</v>
       </c>
       <c r="W42" s="19">
         <f t="shared" si="29"/>
-        <v>4168</v>
+        <v>0</v>
       </c>
       <c r="X42" s="19">
         <f t="shared" si="30"/>
-        <v>5870</v>
+        <v>17610</v>
       </c>
       <c r="Y42" s="19">
         <f t="shared" si="31"/>
-        <v>12224</v>
+        <v>3950</v>
       </c>
       <c r="Z42" s="19">
-        <f t="shared" si="41"/>
-        <v>5000</v>
+        <f t="shared" ref="Z42:Z49" si="53">VLOOKUP(A42,om_table,40,FALSE)</f>
+        <v>12500</v>
       </c>
       <c r="AA42" s="20">
         <f t="shared" si="20"/>
-        <v>28004</v>
+        <v>44137</v>
       </c>
       <c r="AB42" s="39">
-        <f t="shared" si="42"/>
-        <v>0.08</v>
+        <f t="shared" ref="AB42:AB49" si="54">VLOOKUP(A42,om_table,48,FALSE)</f>
+        <v>0.1</v>
       </c>
       <c r="AC42" s="20">
         <f t="shared" si="21"/>
-        <v>2240.3200000000002</v>
+        <v>4413.7</v>
       </c>
       <c r="AD42" s="21">
         <f t="shared" si="32"/>
@@ -8052,7 +8106,7 @@
       </c>
       <c r="AF42" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AG42" s="21">
         <f t="shared" si="25"/>
@@ -8060,19 +8114,19 @@
       </c>
       <c r="AH42" s="22">
         <f t="shared" si="23"/>
-        <v>1744</v>
+        <v>1864</v>
       </c>
       <c r="AI42" s="23">
         <f t="shared" si="22"/>
-        <v>3984.32</v>
+        <v>6277.7</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C43" s="18" t="b">
         <v>1</v>
@@ -8102,31 +8156,27 @@
         <v>362</v>
       </c>
       <c r="L43" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>Cellular Modem</v>
       </c>
-      <c r="M43" s="17" t="str">
-        <f>VLOOKUP(A43,om_table,22,FALSE)</f>
-        <v>BioProbe3</v>
-      </c>
       <c r="O43" s="57" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>Biomark IS1001</v>
       </c>
       <c r="P43" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="49"/>
         <v>2</v>
       </c>
       <c r="Q43" s="17" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="50"/>
         <v>Solar</v>
       </c>
       <c r="R43" s="16">
-        <f t="shared" si="39"/>
-        <v>6</v>
+        <f t="shared" si="51"/>
+        <v>4</v>
       </c>
       <c r="S43" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="52"/>
         <v>4</v>
       </c>
       <c r="T43" s="19">
@@ -8135,7 +8185,7 @@
       </c>
       <c r="U43" s="19">
         <f t="shared" si="27"/>
-        <v>835</v>
+        <v>0</v>
       </c>
       <c r="V43" s="19">
         <f t="shared" si="28"/>
@@ -8151,27 +8201,27 @@
       </c>
       <c r="Y43" s="19">
         <f t="shared" si="31"/>
-        <v>12924</v>
+        <v>12224</v>
       </c>
       <c r="Z43" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="53"/>
         <v>5000</v>
       </c>
       <c r="AA43" s="20">
         <f t="shared" si="20"/>
-        <v>29539</v>
+        <v>28004</v>
       </c>
       <c r="AB43" s="39">
-        <f t="shared" si="42"/>
+        <f t="shared" si="54"/>
         <v>0.08</v>
       </c>
       <c r="AC43" s="20">
         <f t="shared" si="21"/>
-        <v>2363.12</v>
+        <v>2240.3200000000002</v>
       </c>
       <c r="AD43" s="21">
         <f t="shared" si="32"/>
-        <v>546</v>
+        <v>364</v>
       </c>
       <c r="AE43" s="21">
         <f t="shared" si="33"/>
@@ -8187,19 +8237,19 @@
       </c>
       <c r="AH43" s="22">
         <f t="shared" si="23"/>
-        <v>1926</v>
+        <v>1744</v>
       </c>
       <c r="AI43" s="23">
         <f t="shared" si="22"/>
-        <v>4289.12</v>
+        <v>3984.32</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C44" s="18" t="b">
         <v>1</v>
@@ -8229,7 +8279,7 @@
         <v>362</v>
       </c>
       <c r="L44" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>Cellular Modem</v>
       </c>
       <c r="M44" s="17" t="str">
@@ -8237,24 +8287,24 @@
         <v>BioProbe3</v>
       </c>
       <c r="O44" s="57" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>Biomark IS1001</v>
       </c>
       <c r="P44" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="49"/>
         <v>2</v>
       </c>
       <c r="Q44" s="17" t="str">
-        <f t="shared" si="38"/>
-        <v>Grid Power</v>
+        <f t="shared" si="50"/>
+        <v>Solar</v>
       </c>
       <c r="R44" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="51"/>
+        <v>6</v>
+      </c>
+      <c r="S44" s="16">
+        <f t="shared" si="52"/>
         <v>4</v>
-      </c>
-      <c r="S44" s="16">
-        <f t="shared" si="40"/>
-        <v>0</v>
       </c>
       <c r="T44" s="19">
         <f t="shared" si="26"/>
@@ -8278,27 +8328,27 @@
       </c>
       <c r="Y44" s="19">
         <f t="shared" si="31"/>
-        <v>3950</v>
+        <v>12924</v>
       </c>
       <c r="Z44" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="53"/>
         <v>5000</v>
       </c>
       <c r="AA44" s="20">
         <f t="shared" si="20"/>
-        <v>20565</v>
+        <v>29539</v>
       </c>
       <c r="AB44" s="39">
-        <f t="shared" si="42"/>
+        <f t="shared" si="54"/>
         <v>0.08</v>
       </c>
       <c r="AC44" s="20">
         <f t="shared" si="21"/>
-        <v>1645.2</v>
+        <v>2363.12</v>
       </c>
       <c r="AD44" s="21">
         <f t="shared" si="32"/>
-        <v>364</v>
+        <v>546</v>
       </c>
       <c r="AE44" s="21">
         <f t="shared" si="33"/>
@@ -8306,7 +8356,7 @@
       </c>
       <c r="AF44" s="21">
         <f t="shared" si="34"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AG44" s="21">
         <f t="shared" si="25"/>
@@ -8314,19 +8364,19 @@
       </c>
       <c r="AH44" s="22">
         <f t="shared" si="23"/>
-        <v>1864</v>
+        <v>1926</v>
       </c>
       <c r="AI44" s="23">
         <f t="shared" si="22"/>
-        <v>3509.2</v>
+        <v>4289.12</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18" t="b">
         <v>1</v>
@@ -8356,27 +8406,31 @@
         <v>362</v>
       </c>
       <c r="L45" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>Cellular Modem</v>
       </c>
+      <c r="M45" s="17" t="str">
+        <f>VLOOKUP(A45,om_table,22,FALSE)</f>
+        <v>BioProbe3</v>
+      </c>
       <c r="O45" s="57" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>Biomark IS1001</v>
       </c>
       <c r="P45" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="49"/>
         <v>2</v>
       </c>
       <c r="Q45" s="17" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="50"/>
         <v>Grid Power</v>
       </c>
       <c r="R45" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
       <c r="S45" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="T45" s="19">
@@ -8385,7 +8439,7 @@
       </c>
       <c r="U45" s="19">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>835</v>
       </c>
       <c r="V45" s="19">
         <f t="shared" si="28"/>
@@ -8404,20 +8458,20 @@
         <v>3950</v>
       </c>
       <c r="Z45" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="53"/>
         <v>5000</v>
       </c>
       <c r="AA45" s="20">
         <f t="shared" si="20"/>
-        <v>19730</v>
+        <v>20565</v>
       </c>
       <c r="AB45" s="39">
-        <f t="shared" si="42"/>
+        <f t="shared" si="54"/>
         <v>0.08</v>
       </c>
       <c r="AC45" s="20">
         <f t="shared" si="21"/>
-        <v>1578.4</v>
+        <v>1645.2</v>
       </c>
       <c r="AD45" s="21">
         <f t="shared" si="32"/>
@@ -8441,15 +8495,15 @@
       </c>
       <c r="AI45" s="23">
         <f t="shared" si="22"/>
-        <v>3442.4</v>
+        <v>3509.2</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C46" s="18" t="b">
         <v>1</v>
@@ -8461,16 +8515,16 @@
         <v>46</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H46" s="85" t="s">
         <v>369</v>
       </c>
       <c r="I46" s="85" t="s">
-        <v>7</v>
+        <v>370</v>
       </c>
       <c r="J46" s="18" t="s">
         <v>1</v>
@@ -8479,76 +8533,68 @@
         <v>362</v>
       </c>
       <c r="L46" s="17" t="str">
-        <f t="shared" si="35"/>
-        <v>Satellite Modem</v>
-      </c>
-      <c r="M46" s="17" t="str">
-        <f>VLOOKUP(A46,om_table,22,FALSE)</f>
-        <v>BioProbe3</v>
-      </c>
-      <c r="N46" s="17" t="str">
-        <f>VLOOKUP(A46,om_table,20,FALSE)</f>
-        <v>IS1001-MTS</v>
+        <f t="shared" si="47"/>
+        <v>Cellular Modem</v>
       </c>
       <c r="O46" s="57" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>Biomark IS1001</v>
       </c>
       <c r="P46" s="16">
-        <f t="shared" si="37"/>
-        <v>9</v>
+        <f t="shared" si="49"/>
+        <v>2</v>
       </c>
       <c r="Q46" s="17" t="str">
-        <f t="shared" si="38"/>
-        <v>5060 Hybrid TEG</v>
+        <f t="shared" si="50"/>
+        <v>Grid Power</v>
       </c>
       <c r="R46" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
       <c r="S46" s="16">
-        <f t="shared" si="40"/>
-        <v>4</v>
+        <f t="shared" si="52"/>
+        <v>0</v>
       </c>
       <c r="T46" s="19">
         <f t="shared" si="26"/>
-        <v>2000</v>
+        <v>742</v>
       </c>
       <c r="U46" s="19">
         <f t="shared" si="27"/>
-        <v>835</v>
+        <v>0</v>
       </c>
       <c r="V46" s="19">
         <f t="shared" si="28"/>
-        <v>4450</v>
+        <v>0</v>
       </c>
       <c r="W46" s="19">
         <f t="shared" si="29"/>
-        <v>18756</v>
+        <v>4168</v>
       </c>
       <c r="X46" s="19">
         <f t="shared" si="30"/>
-        <v>26415</v>
+        <v>5870</v>
       </c>
       <c r="Y46" s="19">
         <f t="shared" si="31"/>
-        <v>29303</v>
+        <v>3950</v>
       </c>
       <c r="Z46" s="19">
-        <f t="shared" si="41"/>
-        <v>12500</v>
+        <f t="shared" si="53"/>
+        <v>5000</v>
       </c>
       <c r="AA46" s="20">
         <f t="shared" si="20"/>
-        <v>94259</v>
+        <v>19730</v>
       </c>
       <c r="AB46" s="39">
-        <f t="shared" si="42"/>
+        <f t="shared" si="54"/>
         <v>0.08</v>
       </c>
       <c r="AC46" s="20">
         <f t="shared" si="21"/>
-        <v>7540.72</v>
+        <v>1578.4</v>
       </c>
       <c r="AD46" s="21">
         <f t="shared" si="32"/>
@@ -8556,11 +8602,11 @@
       </c>
       <c r="AE46" s="21">
         <f t="shared" si="33"/>
-        <v>1440</v>
+        <v>300</v>
       </c>
       <c r="AF46" s="21">
         <f t="shared" si="34"/>
-        <v>780.19</v>
+        <v>120</v>
       </c>
       <c r="AG46" s="21">
         <f t="shared" si="25"/>
@@ -8568,19 +8614,19 @@
       </c>
       <c r="AH46" s="22">
         <f t="shared" si="23"/>
-        <v>3664.19</v>
+        <v>1864</v>
       </c>
       <c r="AI46" s="23">
         <f t="shared" si="22"/>
-        <v>11204.91</v>
+        <v>3442.4</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C47" s="18" t="b">
         <v>1</v>
@@ -8589,7 +8635,7 @@
         <v>98</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>7</v>
@@ -8610,7 +8656,7 @@
         <v>362</v>
       </c>
       <c r="L47" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>Satellite Modem</v>
       </c>
       <c r="M47" s="17" t="str">
@@ -8619,27 +8665,27 @@
       </c>
       <c r="N47" s="17" t="str">
         <f>VLOOKUP(A47,om_table,20,FALSE)</f>
-        <v>FS1001M</v>
+        <v>IS1001-MTS</v>
       </c>
       <c r="O47" s="57" t="str">
-        <f t="shared" si="36"/>
-        <v>Biomark MUX</v>
+        <f t="shared" si="48"/>
+        <v>Biomark IS1001</v>
       </c>
       <c r="P47" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="49"/>
+        <v>9</v>
+      </c>
+      <c r="Q47" s="17" t="str">
+        <f t="shared" si="50"/>
+        <v>5060 Hybrid TEG</v>
+      </c>
+      <c r="R47" s="16">
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
-      <c r="Q47" s="17" t="str">
-        <f t="shared" si="38"/>
-        <v>5060 TEG</v>
-      </c>
-      <c r="R47" s="16">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
       <c r="S47" s="16">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <f t="shared" si="52"/>
+        <v>4</v>
       </c>
       <c r="T47" s="19">
         <f t="shared" si="26"/>
@@ -8651,39 +8697,39 @@
       </c>
       <c r="V47" s="19">
         <f t="shared" si="28"/>
-        <v>8500</v>
+        <v>4450</v>
       </c>
       <c r="W47" s="19">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>18756</v>
       </c>
       <c r="X47" s="19">
         <f t="shared" si="30"/>
-        <v>11740</v>
+        <v>26415</v>
       </c>
       <c r="Y47" s="19">
         <f t="shared" si="31"/>
-        <v>10479</v>
+        <v>29303</v>
       </c>
       <c r="Z47" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="53"/>
         <v>12500</v>
       </c>
       <c r="AA47" s="20">
         <f t="shared" si="20"/>
-        <v>46054</v>
+        <v>94259</v>
       </c>
       <c r="AB47" s="39">
-        <f t="shared" si="42"/>
-        <v>0.1</v>
+        <f t="shared" si="54"/>
+        <v>0.08</v>
       </c>
       <c r="AC47" s="20">
         <f t="shared" si="21"/>
-        <v>4605.4000000000005</v>
+        <v>7540.72</v>
       </c>
       <c r="AD47" s="21">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="AE47" s="21">
         <f t="shared" si="33"/>
@@ -8691,7 +8737,7 @@
       </c>
       <c r="AF47" s="21">
         <f t="shared" si="34"/>
-        <v>1560.38</v>
+        <v>780.19</v>
       </c>
       <c r="AG47" s="21">
         <f t="shared" si="25"/>
@@ -8699,19 +8745,19 @@
       </c>
       <c r="AH47" s="22">
         <f t="shared" si="23"/>
-        <v>4080.38</v>
+        <v>3664.19</v>
       </c>
       <c r="AI47" s="23">
         <f t="shared" si="22"/>
-        <v>8685.7800000000007</v>
+        <v>11204.91</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C48" s="18" t="b">
         <v>1</v>
@@ -8732,7 +8778,7 @@
         <v>369</v>
       </c>
       <c r="I48" s="85" t="s">
-        <v>363</v>
+        <v>7</v>
       </c>
       <c r="J48" s="18" t="s">
         <v>1</v>
@@ -8741,7 +8787,7 @@
         <v>362</v>
       </c>
       <c r="L48" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>Satellite Modem</v>
       </c>
       <c r="M48" s="17" t="str">
@@ -8753,23 +8799,23 @@
         <v>FS1001M</v>
       </c>
       <c r="O48" s="57" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>Biomark MUX</v>
       </c>
       <c r="P48" s="16">
-        <f t="shared" si="37"/>
-        <v>2</v>
+        <f t="shared" si="49"/>
+        <v>4</v>
       </c>
       <c r="Q48" s="17" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="50"/>
         <v>5060 TEG</v>
       </c>
       <c r="R48" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="S48" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="T48" s="19">
@@ -8790,27 +8836,27 @@
       </c>
       <c r="X48" s="19">
         <f t="shared" si="30"/>
-        <v>5870</v>
+        <v>11740</v>
       </c>
       <c r="Y48" s="19">
         <f t="shared" si="31"/>
         <v>10479</v>
       </c>
       <c r="Z48" s="19">
-        <f t="shared" si="41"/>
-        <v>5000</v>
+        <f t="shared" si="53"/>
+        <v>12500</v>
       </c>
       <c r="AA48" s="20">
         <f t="shared" si="20"/>
-        <v>32684</v>
+        <v>46054</v>
       </c>
       <c r="AB48" s="39">
-        <f t="shared" si="42"/>
+        <f t="shared" si="54"/>
         <v>0.1</v>
       </c>
       <c r="AC48" s="20">
         <f t="shared" si="21"/>
-        <v>3268.4</v>
+        <v>4605.4000000000005</v>
       </c>
       <c r="AD48" s="21">
         <f t="shared" si="32"/>
@@ -8834,15 +8880,15 @@
       </c>
       <c r="AI48" s="23">
         <f t="shared" si="22"/>
-        <v>7348.7800000000007</v>
+        <v>8685.7800000000007</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C49" s="18" t="b">
         <v>1</v>
@@ -8872,7 +8918,7 @@
         <v>362</v>
       </c>
       <c r="L49" s="17" t="str">
-        <f>VLOOKUP(A49,om_table,23,FALSE)</f>
+        <f t="shared" si="47"/>
         <v>Satellite Modem</v>
       </c>
       <c r="M49" s="17" t="str">
@@ -8884,682 +8930,813 @@
         <v>FS1001M</v>
       </c>
       <c r="O49" s="57" t="str">
-        <f>VLOOKUP(A49,om_table,21,FALSE)</f>
+        <f t="shared" si="48"/>
         <v>Biomark MUX</v>
       </c>
       <c r="P49" s="16">
-        <f>VLOOKUP(A49,om_table,30,FALSE)</f>
+        <f t="shared" si="49"/>
+        <v>2</v>
+      </c>
+      <c r="Q49" s="17" t="str">
+        <f t="shared" si="50"/>
+        <v>5060 TEG</v>
+      </c>
+      <c r="R49" s="16">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="S49" s="16">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="T49" s="19">
+        <f t="shared" si="26"/>
+        <v>2000</v>
+      </c>
+      <c r="U49" s="19">
+        <f t="shared" si="27"/>
+        <v>835</v>
+      </c>
+      <c r="V49" s="19">
+        <f t="shared" si="28"/>
+        <v>8500</v>
+      </c>
+      <c r="W49" s="19">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="X49" s="19">
+        <f t="shared" si="30"/>
+        <v>5870</v>
+      </c>
+      <c r="Y49" s="19">
+        <f t="shared" si="31"/>
+        <v>10479</v>
+      </c>
+      <c r="Z49" s="19">
+        <f t="shared" si="53"/>
+        <v>5000</v>
+      </c>
+      <c r="AA49" s="20">
+        <f t="shared" si="20"/>
+        <v>32684</v>
+      </c>
+      <c r="AB49" s="39">
+        <f t="shared" si="54"/>
+        <v>0.1</v>
+      </c>
+      <c r="AC49" s="20">
+        <f t="shared" si="21"/>
+        <v>3268.4</v>
+      </c>
+      <c r="AD49" s="21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AE49" s="21">
+        <f t="shared" si="33"/>
+        <v>1440</v>
+      </c>
+      <c r="AF49" s="21">
+        <f t="shared" si="34"/>
+        <v>1560.38</v>
+      </c>
+      <c r="AG49" s="21">
+        <f t="shared" si="25"/>
+        <v>1080</v>
+      </c>
+      <c r="AH49" s="22">
+        <f t="shared" si="23"/>
+        <v>4080.38</v>
+      </c>
+      <c r="AI49" s="23">
+        <f t="shared" si="22"/>
+        <v>7348.7800000000007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A50" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50" s="85" t="s">
+        <v>369</v>
+      </c>
+      <c r="I50" s="85" t="s">
+        <v>363</v>
+      </c>
+      <c r="J50" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="L50" s="17" t="str">
+        <f>VLOOKUP(A50,om_table,23,FALSE)</f>
+        <v>Satellite Modem</v>
+      </c>
+      <c r="M50" s="17" t="str">
+        <f>VLOOKUP(A50,om_table,22,FALSE)</f>
+        <v>BioProbe3</v>
+      </c>
+      <c r="N50" s="17" t="str">
+        <f>VLOOKUP(A50,om_table,20,FALSE)</f>
+        <v>FS1001M</v>
+      </c>
+      <c r="O50" s="57" t="str">
+        <f>VLOOKUP(A50,om_table,21,FALSE)</f>
+        <v>Biomark MUX</v>
+      </c>
+      <c r="P50" s="16">
+        <f>VLOOKUP(A50,om_table,30,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="Q49" s="17" t="str">
-        <f>VLOOKUP(A49,om_table,9,FALSE)</f>
+      <c r="Q50" s="17" t="str">
+        <f>VLOOKUP(A50,om_table,9,FALSE)</f>
         <v>5060 Hybrid TEG</v>
       </c>
-      <c r="R49" s="16">
-        <f>VLOOKUP(A49,om_table,16,FALSE)</f>
+      <c r="R50" s="16">
+        <f>VLOOKUP(A50,om_table,16,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="S49" s="16">
-        <f>VLOOKUP(A49,om_table,17,FALSE)</f>
+      <c r="S50" s="16">
+        <f>VLOOKUP(A50,om_table,17,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="T49" s="19">
-        <f>VLOOKUP(L49,communication,2,FALSE)</f>
+      <c r="T50" s="19">
+        <f>VLOOKUP(L50,communication,2,FALSE)</f>
         <v>2000</v>
       </c>
-      <c r="U49" s="19">
-        <f>IFERROR(VLOOKUP(M49,datalogger,2,FALSE),0)</f>
+      <c r="U50" s="19">
+        <f>IFERROR(VLOOKUP(M50,datalogger,2,FALSE),0)</f>
         <v>835</v>
       </c>
-      <c r="V49" s="19">
-        <f>IFERROR(VLOOKUP(N49,transceiver,2,FALSE),0)</f>
+      <c r="V50" s="19">
+        <f>IFERROR(VLOOKUP(N50,transceiver,2,FALSE),0)</f>
         <v>8500</v>
       </c>
-      <c r="W49" s="19">
-        <f>VLOOKUP(O49,reader,2,FALSE)*P49</f>
-        <v>0</v>
-      </c>
-      <c r="X49" s="19">
-        <f>P49*antenna_cost</f>
+      <c r="W50" s="19">
+        <f>VLOOKUP(O50,reader,2,FALSE)*P50</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="19">
+        <f>P50*antenna_cost</f>
         <v>14675</v>
       </c>
-      <c r="Y49" s="19">
-        <f>_xlfn.IFS(Q49="Grid Power", 2550, Q49="Grid Power PLC", 3940, Q49="5060 Hybrid TEG", 27903, Q49="5060 TEG", 10479, Q49="5120 TEG", 13874, Q49="Solar", solar_array_cost*S49)+(R49*battery_cost)</f>
+      <c r="Y50" s="19">
+        <f>_xlfn.IFS(Q50="Grid Power", 2550, Q50="Grid Power PLC", 3940, Q50="5060 Hybrid TEG", 27903, Q50="5060 TEG", 10479, Q50="5120 TEG", 13874, Q50="Solar", solar_array_cost*S50)+(R50*battery_cost)</f>
         <v>30003</v>
       </c>
-      <c r="Z49" s="19">
-        <f>VLOOKUP(A49,om_table,40,FALSE)</f>
+      <c r="Z50" s="19">
+        <f>VLOOKUP(A50,om_table,40,FALSE)</f>
         <v>12500</v>
       </c>
-      <c r="AA49" s="20">
-        <f>SUM(T49:Z49)</f>
+      <c r="AA50" s="20">
+        <f>SUM(T50:Z50)</f>
         <v>68513</v>
       </c>
-      <c r="AB49" s="39">
-        <f>VLOOKUP(A49,om_table,48,FALSE)</f>
+      <c r="AB50" s="39">
+        <f>VLOOKUP(A50,om_table,48,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="AC49" s="20">
-        <f>AA49*AB49</f>
+      <c r="AC50" s="20">
+        <f>AA50*AB50</f>
         <v>6851.3</v>
       </c>
-      <c r="AD49" s="21">
-        <f>(R49*battery_replacement)/4</f>
+      <c r="AD50" s="21">
+        <f>(R50*battery_replacement)/4</f>
         <v>546</v>
       </c>
-      <c r="AE49" s="21">
-        <f>VLOOKUP(L49,communication,3,FALSE)</f>
+      <c r="AE50" s="21">
+        <f>VLOOKUP(L50,communication,3,FALSE)</f>
         <v>1440</v>
       </c>
-      <c r="AF49" s="21">
-        <f>VLOOKUP(Q49,power,3,FALSE)</f>
+      <c r="AF50" s="21">
+        <f>VLOOKUP(Q50,power,3,FALSE)</f>
         <v>780.19</v>
       </c>
-      <c r="AG49" s="21">
+      <c r="AG50" s="21">
         <f t="shared" si="18"/>
         <v>1080</v>
       </c>
-      <c r="AH49" s="22">
-        <f>SUM(AD49:AG49)</f>
+      <c r="AH50" s="22">
+        <f>SUM(AD50:AG50)</f>
         <v>3846.19</v>
       </c>
-      <c r="AI49" s="23">
-        <f>AH49+AC49</f>
+      <c r="AI50" s="23">
+        <f>AH50+AC50</f>
         <v>10697.49</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="29"/>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="S52" s="40" t="s">
-        <v>354</v>
-      </c>
-      <c r="T52" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="U52" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="V52" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="W52" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="X52" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y52" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z52" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA52" s="42" t="s">
-        <v>339</v>
-      </c>
-      <c r="AB52" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC52" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="AD52" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE52" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF52" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="AG52" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH52" s="45" t="s">
-        <v>349</v>
-      </c>
-      <c r="AI52" s="46" t="s">
-        <v>345</v>
-      </c>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="29"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="S53" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="T53" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$S53,T$2:T$49,"&lt;&gt;#N/A")</f>
-        <v>39194</v>
-      </c>
-      <c r="U53" s="19">
-        <f>SUMIFS(U$2:U$49,$D$2:$D$49,$S53,U$2:U$49,"&lt;&gt;#N/A")</f>
-        <v>18370</v>
-      </c>
-      <c r="V53" s="19">
-        <f t="shared" ref="V53:Z53" si="43">SUMIFS(V$2:V$49,$D$2:$D$49,$S53,V$2:V$49,"&lt;&gt;#N/A")</f>
-        <v>163900</v>
-      </c>
-      <c r="W53" s="19">
-        <f t="shared" si="43"/>
-        <v>206316</v>
-      </c>
-      <c r="X53" s="19">
-        <f t="shared" si="43"/>
-        <v>484275</v>
-      </c>
-      <c r="Y53" s="19">
-        <f t="shared" si="43"/>
-        <v>300581</v>
-      </c>
-      <c r="Z53" s="19">
-        <f t="shared" si="43"/>
-        <v>312500</v>
-      </c>
-      <c r="AA53" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$S53,AA$2:AA$49,"&lt;&gt;#N/A")</f>
-        <v>1525136</v>
-      </c>
-      <c r="AB53" s="35"/>
-      <c r="AC53" s="35">
-        <f>SUMIFS(AC$2:AC$49,$D$2:$D$49,$S53,AC$2:AC$49,"&lt;&gt;#N/A")</f>
-        <v>135396.36000000002</v>
-      </c>
-      <c r="AD53" s="21">
-        <f>SUMIFS(AD$2:AD$49,$D$2:$D$49,$S53,AD$2:AD$49,"&lt;&gt;#N/A")</f>
-        <v>9282</v>
-      </c>
-      <c r="AE53" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$S53,AE$2:AE$49,"&lt;&gt;#N/A")</f>
-        <v>26580</v>
-      </c>
-      <c r="AF53" s="21">
-        <f t="shared" ref="AF53:AG53" si="44">SUMIFS(AF$2:AF$49,$D$2:$D$49,$S53,AF$2:AF$49,"&lt;&gt;#N/A")</f>
-        <v>22505.100000000002</v>
-      </c>
-      <c r="AG53" s="21">
-        <f t="shared" si="44"/>
-        <v>27000</v>
-      </c>
-      <c r="AH53" s="36">
-        <f>SUMIFS(AH$2:AH$49,$D$2:$D$49,$S53,AH$2:AH$49,"&lt;&gt;#N/A")</f>
-        <v>85367.1</v>
-      </c>
-      <c r="AI53" s="37">
-        <f>SUMIFS(AI$2:AI$49,$D$2:$D$49,$S53,AI$2:AI$49,"&lt;&gt;#N/A")</f>
-        <v>220763.45999999996</v>
+      <c r="S53" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="T53" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="U53" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="V53" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="W53" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="X53" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y53" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z53" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA53" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB53" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC53" s="42" t="s">
+        <v>358</v>
+      </c>
+      <c r="AD53" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE53" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF53" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG53" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH53" s="45" t="s">
+        <v>349</v>
+      </c>
+      <c r="AI53" s="46" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S54" s="32" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="T54" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$S54,T$2:T$49,"&lt;&gt;#N/A")</f>
-        <v>13142</v>
+        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S54,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <v>39194</v>
       </c>
       <c r="U54" s="19">
-        <f t="shared" ref="U54:Z56" si="45">SUMIFS(U$2:U$49,$D$2:$D$49,$S54,U$2:U$49,"&lt;&gt;#N/A")</f>
-        <v>7515</v>
+        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S54,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <v>18370</v>
       </c>
       <c r="V54" s="19">
-        <f t="shared" si="45"/>
-        <v>44100</v>
+        <f t="shared" ref="V54:Z54" si="55">SUMIFS(V$2:V$50,$D$2:$D$50,$S54,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <v>163900</v>
       </c>
       <c r="W54" s="19">
-        <f t="shared" si="45"/>
-        <v>156300</v>
+        <f t="shared" si="55"/>
+        <v>206316</v>
       </c>
       <c r="X54" s="19">
-        <f t="shared" si="45"/>
-        <v>231865</v>
+        <f t="shared" si="55"/>
+        <v>484275</v>
       </c>
       <c r="Y54" s="19">
-        <f t="shared" si="45"/>
-        <v>69606</v>
+        <f t="shared" si="55"/>
+        <v>300581</v>
       </c>
       <c r="Z54" s="19">
-        <f t="shared" si="45"/>
-        <v>112500</v>
+        <f t="shared" si="55"/>
+        <v>312500</v>
       </c>
       <c r="AA54" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$S54,AA$2:AA$49,"&lt;&gt;#N/A")</f>
-        <v>635028</v>
+        <f>SUMIFS(AA$2:AA$50,$D$2:$D$50,$S54,AA$2:AA$50,"&lt;&gt;#N/A")</f>
+        <v>1525136</v>
       </c>
       <c r="AB54" s="35"/>
       <c r="AC54" s="35">
-        <f t="shared" ref="AC54:AI56" si="46">SUMIFS(AC$2:AC$49,$D$2:$D$49,$S54,AC$2:AC$49,"&lt;&gt;#N/A")</f>
-        <v>51532.739999999991</v>
+        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S54,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <v>135396.36000000002</v>
       </c>
       <c r="AD54" s="21">
-        <f t="shared" si="46"/>
-        <v>2912</v>
+        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S54,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <v>9282</v>
       </c>
       <c r="AE54" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$S54,AE$2:AE$49,"&lt;&gt;#N/A")</f>
-        <v>8940</v>
+        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S54,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <v>26580</v>
       </c>
       <c r="AF54" s="21">
-        <f t="shared" si="46"/>
-        <v>6841.51</v>
+        <f t="shared" ref="AF54:AG54" si="56">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S54,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <v>22505.100000000002</v>
       </c>
       <c r="AG54" s="21">
-        <f t="shared" si="46"/>
-        <v>9720</v>
+        <f t="shared" si="56"/>
+        <v>27000</v>
       </c>
       <c r="AH54" s="36">
-        <f t="shared" si="46"/>
-        <v>28413.510000000002</v>
+        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S54,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <v>85367.1</v>
       </c>
       <c r="AI54" s="37">
-        <f t="shared" si="46"/>
-        <v>79946.25</v>
+        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S54,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <v>220763.45999999996</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S55" s="32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T55" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$S55,T$2:T$49,"&lt;&gt;#N/A")</f>
-        <v>6742</v>
+        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S55,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <v>13142</v>
       </c>
       <c r="U55" s="19">
-        <f t="shared" si="45"/>
-        <v>3340</v>
+        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S55,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <v>7515</v>
       </c>
       <c r="V55" s="19">
-        <f t="shared" si="45"/>
-        <v>17800</v>
+        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S55,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <v>44100</v>
       </c>
       <c r="W55" s="19">
-        <f t="shared" si="45"/>
-        <v>83360</v>
+        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S55,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <v>156300</v>
       </c>
       <c r="X55" s="19">
-        <f t="shared" si="45"/>
-        <v>117400</v>
+        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S55,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <v>231865</v>
       </c>
       <c r="Y55" s="19">
-        <f t="shared" si="45"/>
-        <v>63801</v>
+        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S55,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <v>69606</v>
       </c>
       <c r="Z55" s="19">
-        <f t="shared" si="45"/>
-        <v>50000</v>
+        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S55,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <v>112500</v>
       </c>
       <c r="AA55" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$S55,AA$2:AA$49,"&lt;&gt;#N/A")</f>
-        <v>342443</v>
+        <f>SUMIFS(AA$2:AA$50,$D$2:$D$50,$S55,AA$2:AA$50,"&lt;&gt;#N/A")</f>
+        <v>635028</v>
       </c>
       <c r="AB55" s="35"/>
       <c r="AC55" s="35">
-        <f t="shared" si="46"/>
-        <v>27395.439999999999</v>
+        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S55,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <v>51532.739999999991</v>
       </c>
       <c r="AD55" s="21">
-        <f t="shared" si="46"/>
-        <v>1456</v>
+        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S55,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <v>2912</v>
       </c>
       <c r="AE55" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$S55,AE$2:AE$49,"&lt;&gt;#N/A")</f>
-        <v>4620</v>
+        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S55,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <v>8940</v>
       </c>
       <c r="AF55" s="21">
-        <f t="shared" si="46"/>
-        <v>7141.6900000000005</v>
+        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S55,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <v>6841.51</v>
       </c>
       <c r="AG55" s="21">
-        <f t="shared" si="46"/>
-        <v>4320</v>
+        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S55,AG$2:AG$50,"&lt;&gt;#N/A")</f>
+        <v>9720</v>
       </c>
       <c r="AH55" s="36">
-        <f t="shared" si="46"/>
-        <v>17537.690000000002</v>
+        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S55,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <v>28413.510000000002</v>
       </c>
       <c r="AI55" s="37">
-        <f t="shared" si="46"/>
-        <v>44933.13</v>
+        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S55,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <v>79946.25</v>
       </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="S56" s="34" t="s">
-        <v>98</v>
+      <c r="S56" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="T56" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$S56,T$2:T$49,"&lt;&gt;#N/A")</f>
-        <v>11710</v>
+        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S56,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <v>6742</v>
       </c>
       <c r="U56" s="19">
-        <f t="shared" si="45"/>
-        <v>5845</v>
+        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S56,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <v>3340</v>
       </c>
       <c r="V56" s="19">
-        <f t="shared" si="45"/>
-        <v>38450</v>
+        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S56,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <v>17800</v>
       </c>
       <c r="W56" s="19">
-        <f t="shared" si="45"/>
-        <v>35428</v>
+        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S56,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <v>83360</v>
       </c>
       <c r="X56" s="19">
-        <f t="shared" si="45"/>
-        <v>99790</v>
+        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S56,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <v>117400</v>
       </c>
       <c r="Y56" s="19">
-        <f t="shared" si="45"/>
-        <v>117262</v>
+        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S56,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <v>63801</v>
       </c>
       <c r="Z56" s="19">
-        <f t="shared" si="45"/>
-        <v>75000</v>
+        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S56,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <v>50000</v>
       </c>
       <c r="AA56" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$S56,AA$2:AA$49,"&lt;&gt;#N/A")</f>
-        <v>383485</v>
+        <f>SUMIFS(AA$2:AA$50,$D$2:$D$50,$S56,AA$2:AA$50,"&lt;&gt;#N/A")</f>
+        <v>342443</v>
       </c>
       <c r="AB56" s="35"/>
       <c r="AC56" s="35">
-        <f t="shared" si="46"/>
+        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S56,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <v>27395.439999999999</v>
+      </c>
+      <c r="AD56" s="21">
+        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S56,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <v>1456</v>
+      </c>
+      <c r="AE56" s="21">
+        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S56,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <v>4620</v>
+      </c>
+      <c r="AF56" s="21">
+        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S56,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <v>7141.6900000000005</v>
+      </c>
+      <c r="AG56" s="21">
+        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S56,AG$2:AG$50,"&lt;&gt;#N/A")</f>
+        <v>4320</v>
+      </c>
+      <c r="AH56" s="36">
+        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S56,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <v>17537.690000000002</v>
+      </c>
+      <c r="AI56" s="37">
+        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S56,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <v>44933.13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="S57" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="T57" s="19">
+        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S57,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <v>11710</v>
+      </c>
+      <c r="U57" s="19">
+        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S57,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <v>5845</v>
+      </c>
+      <c r="V57" s="19">
+        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S57,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <v>38450</v>
+      </c>
+      <c r="W57" s="19">
+        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S57,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <v>35428</v>
+      </c>
+      <c r="X57" s="19">
+        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S57,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <v>99790</v>
+      </c>
+      <c r="Y57" s="19">
+        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S57,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <v>117262</v>
+      </c>
+      <c r="Z57" s="19">
+        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S57,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <v>75000</v>
+      </c>
+      <c r="AA57" s="35">
+        <f>SUMIFS(AA$2:AA$50,$D$2:$D$50,$S57,AA$2:AA$50,"&lt;&gt;#N/A")</f>
+        <v>383485</v>
+      </c>
+      <c r="AB57" s="35"/>
+      <c r="AC57" s="35">
+        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S57,AC$2:AC$50,"&lt;&gt;#N/A")</f>
         <v>34506.560000000005</v>
       </c>
-      <c r="AD56" s="21">
-        <f t="shared" si="46"/>
+      <c r="AD57" s="21">
+        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S57,AD$2:AD$50,"&lt;&gt;#N/A")</f>
         <v>2912</v>
       </c>
-      <c r="AE56" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$S56,AE$2:AE$49,"&lt;&gt;#N/A")</f>
+      <c r="AE57" s="21">
+        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S57,AE$2:AE$50,"&lt;&gt;#N/A")</f>
         <v>7260</v>
       </c>
-      <c r="AF56" s="21">
-        <f t="shared" si="46"/>
+      <c r="AF57" s="21">
+        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S57,AF$2:AF$50,"&lt;&gt;#N/A")</f>
         <v>5041.1400000000012</v>
       </c>
-      <c r="AG56" s="21">
-        <f t="shared" si="46"/>
+      <c r="AG57" s="21">
+        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S57,AG$2:AG$50,"&lt;&gt;#N/A")</f>
         <v>9720</v>
       </c>
-      <c r="AH56" s="36">
-        <f t="shared" si="46"/>
+      <c r="AH57" s="36">
+        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S57,AH$2:AH$50,"&lt;&gt;#N/A")</f>
         <v>24933.14</v>
       </c>
-      <c r="AI56" s="37">
-        <f t="shared" si="46"/>
+      <c r="AI57" s="37">
+        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S57,AI$2:AI$50,"&lt;&gt;#N/A")</f>
         <v>59439.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="S58" s="33" t="s">
-        <v>355</v>
-      </c>
-      <c r="T58" s="47">
-        <f>T53+T56</f>
-        <v>50904</v>
-      </c>
-      <c r="U58" s="47">
-        <f t="shared" ref="U58:AG58" si="47">U53+U56</f>
-        <v>24215</v>
-      </c>
-      <c r="V58" s="47">
-        <f t="shared" si="47"/>
-        <v>202350</v>
-      </c>
-      <c r="W58" s="47">
-        <f t="shared" si="47"/>
-        <v>241744</v>
-      </c>
-      <c r="X58" s="47">
-        <f t="shared" si="47"/>
-        <v>584065</v>
-      </c>
-      <c r="Y58" s="47">
-        <f t="shared" si="47"/>
-        <v>417843</v>
-      </c>
-      <c r="Z58" s="47">
-        <f t="shared" si="47"/>
-        <v>387500</v>
-      </c>
-      <c r="AA58" s="48">
-        <f>AA53+AA56</f>
-        <v>1908621</v>
-      </c>
-      <c r="AB58" s="48"/>
-      <c r="AC58" s="48">
-        <f>AC53+AC56</f>
-        <v>169902.92</v>
-      </c>
-      <c r="AD58" s="49">
-        <f>AD53+AD56</f>
-        <v>12194</v>
-      </c>
-      <c r="AE58" s="49">
-        <f>AE53+AE56</f>
-        <v>33840</v>
-      </c>
-      <c r="AF58" s="49">
-        <f t="shared" si="47"/>
-        <v>27546.240000000005</v>
-      </c>
-      <c r="AG58" s="49">
-        <f t="shared" si="47"/>
-        <v>36720</v>
-      </c>
-      <c r="AH58" s="50">
-        <f>AH53+AH56</f>
-        <v>110300.24</v>
-      </c>
-      <c r="AI58" s="51">
-        <f>AI53+AI56</f>
-        <v>280203.15999999997</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S59" s="33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="T59" s="47">
-        <f>SUM(T53:T55)</f>
-        <v>59078</v>
+        <f>T54+T57</f>
+        <v>50904</v>
       </c>
       <c r="U59" s="47">
-        <f t="shared" ref="U59:AG59" si="48">SUM(U53:U55)</f>
-        <v>29225</v>
+        <f t="shared" ref="U59:AG59" si="57">U54+U57</f>
+        <v>24215</v>
       </c>
       <c r="V59" s="47">
-        <f t="shared" si="48"/>
-        <v>225800</v>
+        <f t="shared" si="57"/>
+        <v>202350</v>
       </c>
       <c r="W59" s="47">
-        <f t="shared" si="48"/>
-        <v>445976</v>
+        <f t="shared" si="57"/>
+        <v>241744</v>
       </c>
       <c r="X59" s="47">
-        <f t="shared" si="48"/>
-        <v>833540</v>
+        <f t="shared" si="57"/>
+        <v>584065</v>
       </c>
       <c r="Y59" s="47">
-        <f t="shared" si="48"/>
-        <v>433988</v>
+        <f t="shared" si="57"/>
+        <v>417843</v>
       </c>
       <c r="Z59" s="47">
-        <f t="shared" si="48"/>
-        <v>475000</v>
+        <f t="shared" si="57"/>
+        <v>387500</v>
       </c>
       <c r="AA59" s="48">
-        <f>SUM(AA53:AA55)</f>
-        <v>2502607</v>
+        <f>AA54+AA57</f>
+        <v>1908621</v>
       </c>
       <c r="AB59" s="48"/>
       <c r="AC59" s="48">
-        <f>SUM(AC53:AC55)</f>
-        <v>214324.54</v>
+        <f>AC54+AC57</f>
+        <v>169902.92</v>
       </c>
       <c r="AD59" s="49">
-        <f>SUM(AD53:AD55)</f>
-        <v>13650</v>
+        <f>AD54+AD57</f>
+        <v>12194</v>
       </c>
       <c r="AE59" s="49">
-        <f t="shared" si="48"/>
-        <v>40140</v>
+        <f>AE54+AE57</f>
+        <v>33840</v>
       </c>
       <c r="AF59" s="49">
-        <f t="shared" si="48"/>
-        <v>36488.300000000003</v>
+        <f t="shared" si="57"/>
+        <v>27546.240000000005</v>
       </c>
       <c r="AG59" s="49">
-        <f t="shared" si="48"/>
-        <v>41040</v>
+        <f t="shared" si="57"/>
+        <v>36720</v>
       </c>
       <c r="AH59" s="50">
-        <f>SUM(AH53:AH55)</f>
-        <v>131318.30000000002</v>
+        <f>AH54+AH57</f>
+        <v>110300.24</v>
       </c>
       <c r="AI59" s="51">
-        <f>SUM(AI53:AI55)</f>
-        <v>345642.83999999997</v>
+        <f>AI54+AI57</f>
+        <v>280203.15999999997</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S60" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="T60" s="47">
-        <f>T59-T58</f>
-        <v>8174</v>
+        <f>SUM(T54:T56)</f>
+        <v>59078</v>
       </c>
       <c r="U60" s="47">
-        <f t="shared" ref="U60:AG60" si="49">U59-U58</f>
-        <v>5010</v>
+        <f t="shared" ref="U60:AG60" si="58">SUM(U54:U56)</f>
+        <v>29225</v>
       </c>
       <c r="V60" s="47">
-        <f t="shared" si="49"/>
-        <v>23450</v>
+        <f t="shared" si="58"/>
+        <v>225800</v>
       </c>
       <c r="W60" s="47">
-        <f t="shared" si="49"/>
-        <v>204232</v>
+        <f t="shared" si="58"/>
+        <v>445976</v>
       </c>
       <c r="X60" s="47">
-        <f t="shared" si="49"/>
-        <v>249475</v>
+        <f t="shared" si="58"/>
+        <v>833540</v>
       </c>
       <c r="Y60" s="47">
-        <f t="shared" si="49"/>
-        <v>16145</v>
+        <f t="shared" si="58"/>
+        <v>433988</v>
       </c>
       <c r="Z60" s="47">
-        <f t="shared" si="49"/>
-        <v>87500</v>
+        <f t="shared" si="58"/>
+        <v>475000</v>
       </c>
       <c r="AA60" s="48">
-        <f>AA59-AA58</f>
-        <v>593986</v>
+        <f>SUM(AA54:AA56)</f>
+        <v>2502607</v>
       </c>
       <c r="AB60" s="48"/>
       <c r="AC60" s="48">
-        <f>AC59-AC58</f>
-        <v>44421.619999999995</v>
+        <f>SUM(AC54:AC56)</f>
+        <v>214324.54</v>
       </c>
       <c r="AD60" s="49">
-        <f>AD59-AD58</f>
-        <v>1456</v>
+        <f>SUM(AD54:AD56)</f>
+        <v>13650</v>
       </c>
       <c r="AE60" s="49">
-        <f t="shared" si="49"/>
-        <v>6300</v>
+        <f t="shared" si="58"/>
+        <v>40140</v>
       </c>
       <c r="AF60" s="49">
-        <f t="shared" si="49"/>
-        <v>8942.0599999999977</v>
+        <f t="shared" si="58"/>
+        <v>36488.300000000003</v>
       </c>
       <c r="AG60" s="49">
-        <f t="shared" si="49"/>
-        <v>4320</v>
+        <f t="shared" si="58"/>
+        <v>41040</v>
       </c>
       <c r="AH60" s="50">
-        <f>AH59-AH58</f>
-        <v>21018.060000000012</v>
+        <f>SUM(AH54:AH56)</f>
+        <v>131318.30000000002</v>
       </c>
       <c r="AI60" s="51">
-        <f>AI59-AI58</f>
-        <v>65439.679999999993</v>
+        <f>SUM(AI54:AI56)</f>
+        <v>345642.83999999997</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="S61" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="T61" s="47">
+        <f>T60-T59</f>
+        <v>8174</v>
+      </c>
+      <c r="U61" s="47">
+        <f t="shared" ref="U61:AG61" si="59">U60-U59</f>
+        <v>5010</v>
+      </c>
+      <c r="V61" s="47">
+        <f t="shared" si="59"/>
+        <v>23450</v>
+      </c>
+      <c r="W61" s="47">
+        <f t="shared" si="59"/>
+        <v>204232</v>
+      </c>
+      <c r="X61" s="47">
+        <f t="shared" si="59"/>
+        <v>249475</v>
+      </c>
+      <c r="Y61" s="47">
+        <f t="shared" si="59"/>
+        <v>16145</v>
+      </c>
+      <c r="Z61" s="47">
+        <f t="shared" si="59"/>
+        <v>87500</v>
+      </c>
+      <c r="AA61" s="48">
+        <f>AA60-AA59</f>
+        <v>593986</v>
+      </c>
+      <c r="AB61" s="48"/>
+      <c r="AC61" s="48">
+        <f>AC60-AC59</f>
+        <v>44421.619999999995</v>
+      </c>
+      <c r="AD61" s="49">
+        <f>AD60-AD59</f>
+        <v>1456</v>
+      </c>
+      <c r="AE61" s="49">
+        <f t="shared" si="59"/>
+        <v>6300</v>
+      </c>
+      <c r="AF61" s="49">
+        <f t="shared" si="59"/>
+        <v>8942.0599999999977</v>
+      </c>
+      <c r="AG61" s="49">
+        <f t="shared" si="59"/>
+        <v>4320</v>
+      </c>
+      <c r="AH61" s="50">
+        <f>AH60-AH59</f>
+        <v>21018.060000000012</v>
+      </c>
+      <c r="AI61" s="51">
+        <f>AI60-AI59</f>
+        <v>65439.679999999993</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="S62" s="33" t="s">
         <v>359</v>
       </c>
-      <c r="T61" s="52">
-        <f>T60/T58</f>
+      <c r="T62" s="52">
+        <f>T61/T59</f>
         <v>0.16057677196291056</v>
       </c>
-      <c r="U61" s="52">
-        <f t="shared" ref="U61:AG61" si="50">U60/U58</f>
+      <c r="U62" s="52">
+        <f t="shared" ref="U62:AG62" si="60">U61/U59</f>
         <v>0.20689655172413793</v>
       </c>
-      <c r="V61" s="52">
-        <f t="shared" si="50"/>
+      <c r="V62" s="52">
+        <f t="shared" si="60"/>
         <v>0.11588831233012108</v>
       </c>
-      <c r="W61" s="52">
-        <f t="shared" si="50"/>
+      <c r="W62" s="52">
+        <f t="shared" si="60"/>
         <v>0.84482758620689657</v>
       </c>
-      <c r="X61" s="52">
-        <f t="shared" si="50"/>
+      <c r="X62" s="52">
+        <f t="shared" si="60"/>
         <v>0.42713567839195982</v>
       </c>
-      <c r="Y61" s="52">
-        <f t="shared" si="50"/>
+      <c r="Y62" s="52">
+        <f t="shared" si="60"/>
         <v>3.863891461625539E-2</v>
       </c>
-      <c r="Z61" s="52">
-        <f t="shared" si="50"/>
+      <c r="Z62" s="52">
+        <f t="shared" si="60"/>
         <v>0.22580645161290322</v>
       </c>
-      <c r="AA61" s="53">
-        <f>AA60/AA58</f>
+      <c r="AA62" s="53">
+        <f>AA61/AA59</f>
         <v>0.31121212645150609</v>
       </c>
-      <c r="AB61" s="53"/>
-      <c r="AC61" s="53">
-        <f>AC60/AC58</f>
+      <c r="AB62" s="53"/>
+      <c r="AC62" s="53">
+        <f>AC61/AC59</f>
         <v>0.26145295207404318</v>
       </c>
-      <c r="AD61" s="54">
-        <f>AD60/AD58</f>
+      <c r="AD62" s="54">
+        <f>AD61/AD59</f>
         <v>0.11940298507462686</v>
       </c>
-      <c r="AE61" s="54">
-        <f t="shared" si="50"/>
+      <c r="AE62" s="54">
+        <f t="shared" si="60"/>
         <v>0.18617021276595744</v>
       </c>
-      <c r="AF61" s="54">
-        <f t="shared" si="50"/>
+      <c r="AF62" s="54">
+        <f t="shared" si="60"/>
         <v>0.32461998443344703</v>
       </c>
-      <c r="AG61" s="54">
-        <f t="shared" si="50"/>
+      <c r="AG62" s="54">
+        <f t="shared" si="60"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="AH61" s="55">
-        <f>AH60/AH58</f>
+      <c r="AH62" s="55">
+        <f>AH61/AH59</f>
         <v>0.19055316652076199</v>
       </c>
-      <c r="AI61" s="56">
-        <f>AI60/AI58</f>
+      <c r="AI62" s="56">
+        <f>AI61/AI59</f>
         <v>0.23354369022819013</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:K50">
-    <sortCondition ref="D28:D50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:K51">
+    <sortCondition ref="D28:D51"/>
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
folded ACM into imp plan; saving o&m costs
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20241213.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20241213.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3595E02D-847A-43BC-A6F6-844C82AF2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167DDC30-9CF6-437E-8820-9591AF9E5571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="391">
   <si>
     <t>WDFW</t>
   </si>
@@ -2497,7 +2497,7 @@
   <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2672,7 +2672,9 @@
       <c r="B8" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="100" t="s">
+        <v>379</v>
+      </c>
       <c r="D8" s="100" t="s">
         <v>385</v>
       </c>
@@ -9211,31 +9213,31 @@
         <v>99</v>
       </c>
       <c r="T54" s="19">
-        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S54,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="T54:U57" si="55">SUMIFS(T$2:T$50,$D$2:$D$50,$S54,T$2:T$50,"&lt;&gt;#N/A")</f>
         <v>39194</v>
       </c>
       <c r="U54" s="19">
-        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S54,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>18370</v>
       </c>
       <c r="V54" s="19">
-        <f t="shared" ref="V54:Z54" si="55">SUMIFS(V$2:V$50,$D$2:$D$50,$S54,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="V54:Z54" si="56">SUMIFS(V$2:V$50,$D$2:$D$50,$S54,V$2:V$50,"&lt;&gt;#N/A")</f>
         <v>163900</v>
       </c>
       <c r="W54" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>206316</v>
       </c>
       <c r="X54" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>484275</v>
       </c>
       <c r="Y54" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>300581</v>
       </c>
       <c r="Z54" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>312500</v>
       </c>
       <c r="AA54" s="35">
@@ -9244,31 +9246,31 @@
       </c>
       <c r="AB54" s="35"/>
       <c r="AC54" s="35">
-        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S54,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AC54:AE57" si="57">SUMIFS(AC$2:AC$50,$D$2:$D$50,$S54,AC$2:AC$50,"&lt;&gt;#N/A")</f>
         <v>135396.36000000002</v>
       </c>
       <c r="AD54" s="21">
-        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S54,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>9282</v>
       </c>
       <c r="AE54" s="21">
-        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S54,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>26580</v>
       </c>
       <c r="AF54" s="21">
-        <f t="shared" ref="AF54:AG54" si="56">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S54,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AF54:AG54" si="58">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S54,AF$2:AF$50,"&lt;&gt;#N/A")</f>
         <v>22505.100000000002</v>
       </c>
       <c r="AG54" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>27000</v>
       </c>
       <c r="AH54" s="36">
-        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S54,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AH54:AI57" si="59">SUMIFS(AH$2:AH$50,$D$2:$D$50,$S54,AH$2:AH$50,"&lt;&gt;#N/A")</f>
         <v>85367.1</v>
       </c>
       <c r="AI54" s="37">
-        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S54,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>220763.45999999996</v>
       </c>
     </row>
@@ -9277,31 +9279,31 @@
         <v>94</v>
       </c>
       <c r="T55" s="19">
-        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S55,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>13142</v>
       </c>
       <c r="U55" s="19">
-        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S55,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>7515</v>
       </c>
       <c r="V55" s="19">
-        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S55,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="V55:Z57" si="60">SUMIFS(V$2:V$50,$D$2:$D$50,$S55,V$2:V$50,"&lt;&gt;#N/A")</f>
         <v>44100</v>
       </c>
       <c r="W55" s="19">
-        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S55,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>156300</v>
       </c>
       <c r="X55" s="19">
-        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S55,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>231865</v>
       </c>
       <c r="Y55" s="19">
-        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S55,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>69606</v>
       </c>
       <c r="Z55" s="19">
-        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S55,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>112500</v>
       </c>
       <c r="AA55" s="35">
@@ -9310,31 +9312,31 @@
       </c>
       <c r="AB55" s="35"/>
       <c r="AC55" s="35">
-        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S55,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>51532.739999999991</v>
       </c>
       <c r="AD55" s="21">
-        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S55,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>2912</v>
       </c>
       <c r="AE55" s="21">
-        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S55,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>8940</v>
       </c>
       <c r="AF55" s="21">
-        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S55,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AF55:AG57" si="61">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S55,AF$2:AF$50,"&lt;&gt;#N/A")</f>
         <v>6841.51</v>
       </c>
       <c r="AG55" s="21">
-        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S55,AG$2:AG$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="61"/>
         <v>9720</v>
       </c>
       <c r="AH55" s="36">
-        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S55,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>28413.510000000002</v>
       </c>
       <c r="AI55" s="37">
-        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S55,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>79946.25</v>
       </c>
     </row>
@@ -9343,31 +9345,31 @@
         <v>97</v>
       </c>
       <c r="T56" s="19">
-        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S56,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>6742</v>
       </c>
       <c r="U56" s="19">
-        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S56,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>3340</v>
       </c>
       <c r="V56" s="19">
-        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S56,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>17800</v>
       </c>
       <c r="W56" s="19">
-        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S56,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>83360</v>
       </c>
       <c r="X56" s="19">
-        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S56,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>117400</v>
       </c>
       <c r="Y56" s="19">
-        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S56,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>63801</v>
       </c>
       <c r="Z56" s="19">
-        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S56,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>50000</v>
       </c>
       <c r="AA56" s="35">
@@ -9376,31 +9378,31 @@
       </c>
       <c r="AB56" s="35"/>
       <c r="AC56" s="35">
-        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S56,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>27395.439999999999</v>
       </c>
       <c r="AD56" s="21">
-        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S56,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>1456</v>
       </c>
       <c r="AE56" s="21">
-        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S56,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>4620</v>
       </c>
       <c r="AF56" s="21">
-        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S56,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="61"/>
         <v>7141.6900000000005</v>
       </c>
       <c r="AG56" s="21">
-        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S56,AG$2:AG$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="61"/>
         <v>4320</v>
       </c>
       <c r="AH56" s="36">
-        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S56,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>17537.690000000002</v>
       </c>
       <c r="AI56" s="37">
-        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S56,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>44933.13</v>
       </c>
     </row>
@@ -9409,31 +9411,31 @@
         <v>98</v>
       </c>
       <c r="T57" s="19">
-        <f>SUMIFS(T$2:T$50,$D$2:$D$50,$S57,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>11710</v>
       </c>
       <c r="U57" s="19">
-        <f>SUMIFS(U$2:U$50,$D$2:$D$50,$S57,U$2:U$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="55"/>
         <v>5845</v>
       </c>
       <c r="V57" s="19">
-        <f>SUMIFS(V$2:V$50,$D$2:$D$50,$S57,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>38450</v>
       </c>
       <c r="W57" s="19">
-        <f>SUMIFS(W$2:W$50,$D$2:$D$50,$S57,W$2:W$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>35428</v>
       </c>
       <c r="X57" s="19">
-        <f>SUMIFS(X$2:X$50,$D$2:$D$50,$S57,X$2:X$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>99790</v>
       </c>
       <c r="Y57" s="19">
-        <f>SUMIFS(Y$2:Y$50,$D$2:$D$50,$S57,Y$2:Y$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>117262</v>
       </c>
       <c r="Z57" s="19">
-        <f>SUMIFS(Z$2:Z$50,$D$2:$D$50,$S57,Z$2:Z$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="60"/>
         <v>75000</v>
       </c>
       <c r="AA57" s="35">
@@ -9442,31 +9444,31 @@
       </c>
       <c r="AB57" s="35"/>
       <c r="AC57" s="35">
-        <f>SUMIFS(AC$2:AC$50,$D$2:$D$50,$S57,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>34506.560000000005</v>
       </c>
       <c r="AD57" s="21">
-        <f>SUMIFS(AD$2:AD$50,$D$2:$D$50,$S57,AD$2:AD$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>2912</v>
       </c>
       <c r="AE57" s="21">
-        <f>SUMIFS(AE$2:AE$50,$D$2:$D$50,$S57,AE$2:AE$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="57"/>
         <v>7260</v>
       </c>
       <c r="AF57" s="21">
-        <f>SUMIFS(AF$2:AF$50,$D$2:$D$50,$S57,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="61"/>
         <v>5041.1400000000012</v>
       </c>
       <c r="AG57" s="21">
-        <f>SUMIFS(AG$2:AG$50,$D$2:$D$50,$S57,AG$2:AG$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="61"/>
         <v>9720</v>
       </c>
       <c r="AH57" s="36">
-        <f>SUMIFS(AH$2:AH$50,$D$2:$D$50,$S57,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>24933.14</v>
       </c>
       <c r="AI57" s="37">
-        <f>SUMIFS(AI$2:AI$50,$D$2:$D$50,$S57,AI$2:AI$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="59"/>
         <v>59439.7</v>
       </c>
     </row>
@@ -9479,27 +9481,27 @@
         <v>50904</v>
       </c>
       <c r="U59" s="47">
-        <f t="shared" ref="U59:AG59" si="57">U54+U57</f>
+        <f t="shared" ref="U59:AG59" si="62">U54+U57</f>
         <v>24215</v>
       </c>
       <c r="V59" s="47">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>202350</v>
       </c>
       <c r="W59" s="47">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>241744</v>
       </c>
       <c r="X59" s="47">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>584065</v>
       </c>
       <c r="Y59" s="47">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>417843</v>
       </c>
       <c r="Z59" s="47">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>387500</v>
       </c>
       <c r="AA59" s="48">
@@ -9520,11 +9522,11 @@
         <v>33840</v>
       </c>
       <c r="AF59" s="49">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>27546.240000000005</v>
       </c>
       <c r="AG59" s="49">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>36720</v>
       </c>
       <c r="AH59" s="50">
@@ -9545,27 +9547,27 @@
         <v>59078</v>
       </c>
       <c r="U60" s="47">
-        <f t="shared" ref="U60:AG60" si="58">SUM(U54:U56)</f>
+        <f t="shared" ref="U60:AG60" si="63">SUM(U54:U56)</f>
         <v>29225</v>
       </c>
       <c r="V60" s="47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>225800</v>
       </c>
       <c r="W60" s="47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>445976</v>
       </c>
       <c r="X60" s="47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>833540</v>
       </c>
       <c r="Y60" s="47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>433988</v>
       </c>
       <c r="Z60" s="47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>475000</v>
       </c>
       <c r="AA60" s="48">
@@ -9582,15 +9584,15 @@
         <v>13650</v>
       </c>
       <c r="AE60" s="49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>40140</v>
       </c>
       <c r="AF60" s="49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>36488.300000000003</v>
       </c>
       <c r="AG60" s="49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>41040</v>
       </c>
       <c r="AH60" s="50">
@@ -9611,27 +9613,27 @@
         <v>8174</v>
       </c>
       <c r="U61" s="47">
-        <f t="shared" ref="U61:AG61" si="59">U60-U59</f>
+        <f t="shared" ref="U61:AG61" si="64">U60-U59</f>
         <v>5010</v>
       </c>
       <c r="V61" s="47">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>23450</v>
       </c>
       <c r="W61" s="47">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>204232</v>
       </c>
       <c r="X61" s="47">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>249475</v>
       </c>
       <c r="Y61" s="47">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>16145</v>
       </c>
       <c r="Z61" s="47">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>87500</v>
       </c>
       <c r="AA61" s="48">
@@ -9648,15 +9650,15 @@
         <v>1456</v>
       </c>
       <c r="AE61" s="49">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>6300</v>
       </c>
       <c r="AF61" s="49">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>8942.0599999999977</v>
       </c>
       <c r="AG61" s="49">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>4320</v>
       </c>
       <c r="AH61" s="50">
@@ -9677,27 +9679,27 @@
         <v>0.16057677196291056</v>
       </c>
       <c r="U62" s="52">
-        <f t="shared" ref="U62:AG62" si="60">U61/U59</f>
+        <f t="shared" ref="U62:AG62" si="65">U61/U59</f>
         <v>0.20689655172413793</v>
       </c>
       <c r="V62" s="52">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.11588831233012108</v>
       </c>
       <c r="W62" s="52">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.84482758620689657</v>
       </c>
       <c r="X62" s="52">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.42713567839195982</v>
       </c>
       <c r="Y62" s="52">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>3.863891461625539E-2</v>
       </c>
       <c r="Z62" s="52">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="AA62" s="53">
@@ -9714,15 +9716,15 @@
         <v>0.11940298507462686</v>
       </c>
       <c r="AE62" s="54">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.18617021276595744</v>
       </c>
       <c r="AF62" s="54">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.32461998443344703</v>
       </c>
       <c r="AG62" s="54">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="AH62" s="55">

</xml_diff>